<commit_message>
3. Find the Kth max and min element of an array
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EE3DEA-8ECA-4D14-9A33-CB7034375DF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEB5F80-B176-44CE-9D77-B4B005C4A85D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1952,8 +1952,8 @@
       <c r="C9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>4</v>
+      <c r="D9" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="21">

</xml_diff>

<commit_message>
5. Move all the negative elements to one side of the array
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEB5F80-B176-44CE-9D77-B4B005C4A85D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB18BF2D-90E4-447D-ACC5-3D1F5E2DB0D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1864,7 +1864,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1966,8 +1966,8 @@
       <c r="C10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>4</v>
+      <c r="D10" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="21">

</xml_diff>

<commit_message>
6. Find the Union and Intersection of the two sorted arrays.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB18BF2D-90E4-447D-ACC5-3D1F5E2DB0D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF95F697-4415-49D1-986F-BD90ED92ADC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,13 +1863,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="19.375" customWidth="1"/>
     <col min="3" max="3" width="103.75" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
@@ -1980,8 +1981,8 @@
       <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>4</v>
+      <c r="D11" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="21">

</xml_diff>

<commit_message>
8. find Largest sum contiguous Subarray [V. IMP]
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF95F697-4415-49D1-986F-BD90ED92ADC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF0DF90-3BEC-4747-9A53-F9DCE96CCC17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1995,8 +1995,8 @@
       <c r="C12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>4</v>
+      <c r="D12" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21">
@@ -2009,8 +2009,8 @@
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>4</v>
+      <c r="D13" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="21">

</xml_diff>

<commit_message>
1471B - Strange List
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF0DF90-3BEC-4747-9A53-F9DCE96CCC17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499F22A4-B121-469E-85DD-561C7B726A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1492,7 +1492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1502,6 +1502,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1519,7 +1525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1544,6 +1550,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1864,7 +1873,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2023,7 +2032,7 @@
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2037,7 +2046,7 @@
       <c r="C15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2051,7 +2060,7 @@
       <c r="C16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="12" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1421B - Putting Bricks in the Wall
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499F22A4-B121-469E-85DD-561C7B726A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6353DF4E-43FB-473C-96CC-1CE94CBF0BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2074,7 +2074,7 @@
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2088,7 +2088,7 @@
       <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2102,7 +2102,7 @@
       <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2116,7 +2116,7 @@
       <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="12" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
17. Best time to buy and Sell stock
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6353DF4E-43FB-473C-96CC-1CE94CBF0BDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9631FC34-7377-48BC-A35E-8020EE10EF7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2130,7 +2130,7 @@
       <c r="C21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2144,8 +2144,8 @@
       <c r="C22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>4</v>
+      <c r="D22" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="21">

</xml_diff>

<commit_message>
18. find all pairs on integer array whose sum is equal to given number
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9631FC34-7377-48BC-A35E-8020EE10EF7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1166B3F0-418E-4AAF-9CA4-0F10C9F49957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2158,8 +2158,8 @@
       <c r="C23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>4</v>
+      <c r="D23" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="21">

</xml_diff>

<commit_message>
19. find common elements In 3 sorted arrays
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1166B3F0-418E-4AAF-9CA4-0F10C9F49957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789AD34E-63C7-424D-85B1-D4776A050450}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2172,8 +2172,8 @@
       <c r="C24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>4</v>
+      <c r="D24" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="21">

</xml_diff>

<commit_message>
1541B - Pleasant Pairs
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789AD34E-63C7-424D-85B1-D4776A050450}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7315A85-FA70-4687-8335-D9534006EF74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2186,7 +2186,7 @@
       <c r="C25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="12" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
21. Find if there is any subarray with sum equal to 0.cpp
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7315A85-FA70-4687-8335-D9534006EF74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F058D48-B41D-435A-9972-D0C86F60B870}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2200,8 +2200,8 @@
       <c r="C26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>4</v>
+      <c r="D26" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21">

</xml_diff>

<commit_message>
24. Find longest coinsecutive subsequence
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F058D48-B41D-435A-9972-D0C86F60B870}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC43AF1-A5B0-4178-B494-169DC16B17E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1492,7 +1492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1511,6 +1511,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1525,7 +1531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1553,6 +1559,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1872,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2214,7 +2223,7 @@
       <c r="C27" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="13" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2228,7 +2237,7 @@
       <c r="C28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="12" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2242,8 +2251,8 @@
       <c r="C29" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>4</v>
+      <c r="D29" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="21">

</xml_diff>

<commit_message>
25. Given an array of size n and a number k, fin all elements that appear more than n by k  times.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC43AF1-A5B0-4178-B494-169DC16B17E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D2C7A3-DC3C-465A-B44D-9BF70E651E87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2265,8 +2265,8 @@
       <c r="C30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>4</v>
+      <c r="D30" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="21">

</xml_diff>

<commit_message>
1539C - Stable Groups
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D2C7A3-DC3C-465A-B44D-9BF70E651E87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93853CE7-1154-4EDB-ACED-352A27088B18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
9. Minimise the maximum difference between heights [V.IMP]
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93853CE7-1154-4EDB-ACED-352A27088B18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF70D98-4916-4FA9-88B7-80A4E9FA9B1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
1497C1 - k-LCM (easy version)
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF70D98-4916-4FA9-88B7-80A4E9FA9B1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC4BDBC-B471-4D7B-97A3-E6CA473553D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2042,7 +2042,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21">

</xml_diff>

<commit_message>
11. find duplicate in an array of N+1 Integers
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC4BDBC-B471-4D7B-97A3-E6CA473553D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014ACC2F-849A-4F56-B321-1CE07DA18E5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2070,7 +2070,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="21">
@@ -2098,7 +2098,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="21">
@@ -2112,7 +2112,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="21">

</xml_diff>

<commit_message>
12. Merge 2 sorted arrays without using Extra space.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{014ACC2F-849A-4F56-B321-1CE07DA18E5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B58C1B-39E8-4863-B9F9-CBFF6B69C7AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2084,7 +2084,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21">

</xml_diff>

<commit_message>
162. Level Order Traversal
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47DB7B4-8628-43DD-8917-62C0FC4ABAC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18FA39B-7AC0-4D9A-AD4B-34C7ED395229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="D168" sqref="D168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4183,8 +4183,8 @@
       <c r="C167" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D167" s="4" t="s">
-        <v>4</v>
+      <c r="D167" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="21">

</xml_diff>

<commit_message>
163. Reverse Level Order Traversal
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18FA39B-7AC0-4D9A-AD4B-34C7ED395229}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A9B1FF-79BA-4104-A852-0239492E1352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+      <selection activeCell="C167" sqref="C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4197,8 +4197,8 @@
       <c r="C168" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D168" s="4" t="s">
-        <v>4</v>
+      <c r="D168" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="21">

</xml_diff>

<commit_message>
164. Height of a Tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A9B1FF-79BA-4104-A852-0239492E1352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D958C5-C28A-42FD-AF8C-7F94890A5072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="C167" sqref="C167"/>
+      <selection activeCell="D169" sqref="D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4211,8 +4211,8 @@
       <c r="C169" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D169" s="4" t="s">
-        <v>4</v>
+      <c r="D169" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="21">

</xml_diff>

<commit_message>
165. Diameter of a Tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D958C5-C28A-42FD-AF8C-7F94890A5072}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B26C8A9-0680-4D0C-967E-D2A1CF65A42E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="D169" sqref="D169"/>
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4225,8 +4225,8 @@
       <c r="C170" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D170" s="4" t="s">
-        <v>4</v>
+      <c r="D170" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="21">

</xml_diff>

<commit_message>
166. Mirror of a Tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B26C8A9-0680-4D0C-967E-D2A1CF65A42E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB1D5B-4CC7-44F6-959D-D45EA2331297}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4239,8 +4239,8 @@
       <c r="C171" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="D171" s="4" t="s">
-        <v>4</v>
+      <c r="D171" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="21">

</xml_diff>

<commit_message>
167. Inorder Traversal of a tree both using recursion and Iteration
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DB1D5B-4CC7-44F6-959D-D45EA2331297}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A780E87-2351-45D6-A800-90731D492EB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="D171" sqref="D171"/>
+      <selection activeCell="C172" sqref="C172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4253,8 +4253,8 @@
       <c r="C172" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D172" s="4" t="s">
-        <v>4</v>
+      <c r="D172" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="21">
@@ -4267,8 +4267,8 @@
       <c r="C173" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="D173" s="4" t="s">
-        <v>4</v>
+      <c r="D173" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="21">
@@ -4281,8 +4281,8 @@
       <c r="C174" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D174" s="4" t="s">
-        <v>4</v>
+      <c r="D174" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="21">

</xml_diff>

<commit_message>
170. Left View of Binary Tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A780E87-2351-45D6-A800-90731D492EB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF2F273-A1F4-4AB7-83E4-3918014D8F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="C172" sqref="C172"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="D176" sqref="D176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4295,8 +4295,8 @@
       <c r="C175" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D175" s="4" t="s">
-        <v>4</v>
+      <c r="D175" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="21">
@@ -4309,8 +4309,8 @@
       <c r="C176" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D176" s="4" t="s">
-        <v>4</v>
+      <c r="D176" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="21">

</xml_diff>

<commit_message>
172. Top VIew of Binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF2F273-A1F4-4AB7-83E4-3918014D8F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65041229-D4A4-44FC-8BD4-ABBE782EEB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="D176" sqref="D176"/>
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4323,8 +4323,8 @@
       <c r="C177" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="D177" s="4" t="s">
-        <v>4</v>
+      <c r="D177" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:4" ht="21">
@@ -4337,8 +4337,8 @@
       <c r="C178" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="D178" s="4" t="s">
-        <v>4</v>
+      <c r="D178" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:4" ht="21">

</xml_diff>

<commit_message>
1472D - Even-Odd Game
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65041229-D4A4-44FC-8BD4-ABBE782EEB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47770EB6-480A-43A0-B18F-1982E3346F53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="D178" sqref="D178"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="D179" sqref="D179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
174. Zig-Zag traversal of a binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47770EB6-480A-43A0-B18F-1982E3346F53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A52E59-5D08-4699-8833-F524C6BAC66F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="D179" sqref="D179"/>
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4351,8 +4351,8 @@
       <c r="C179" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="D179" s="4" t="s">
-        <v>4</v>
+      <c r="D179" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:4" ht="21">

</xml_diff>

<commit_message>
175. Check if a Binary Tree is Balanced or not
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A52E59-5D08-4699-8833-F524C6BAC66F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24210591-5753-4FF5-ACAB-C2E152953917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="C179" sqref="C179"/>
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4365,8 +4365,8 @@
       <c r="C180" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="D180" s="4" t="s">
-        <v>4</v>
+      <c r="D180" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:4" ht="21">

</xml_diff>

<commit_message>
176. Diagonal Traversal of a Binary Tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24210591-5753-4FF5-ACAB-C2E152953917}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8035D4-3823-4AE5-B2F9-0AA7CD640C1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+      <selection activeCell="D181" sqref="D181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4379,8 +4379,8 @@
       <c r="C181" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="D181" s="4" t="s">
-        <v>4</v>
+      <c r="D181" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:4" ht="21">

</xml_diff>

<commit_message>
177. Boundary Traversal of binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8035D4-3823-4AE5-B2F9-0AA7CD640C1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293CA4E2-CB6F-4D8B-A28B-D99069316057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="D181" sqref="D181"/>
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4393,8 +4393,8 @@
       <c r="C182" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D182" s="4" t="s">
-        <v>4</v>
+      <c r="D182" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:4" ht="21">

</xml_diff>

<commit_message>
180. Convert Binary tree into Sum tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293CA4E2-CB6F-4D8B-A28B-D99069316057}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0DF62B-F393-423A-AA27-2D8ABFF5C73D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+      <selection activeCell="C185" sqref="C185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4435,8 +4435,8 @@
       <c r="C185" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="D185" s="4" t="s">
-        <v>4</v>
+      <c r="D185" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:4" ht="21">

</xml_diff>

<commit_message>
1366A - Shovels and Swords
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0DF62B-F393-423A-AA27-2D8ABFF5C73D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAEE5AE-92B9-4A81-BC5E-383E1285C3F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="C185" sqref="C185"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
178. Construct Binary Tree from String with Bracket Representation
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAEE5AE-92B9-4A81-BC5E-383E1285C3F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4A13C2-04CC-4AB7-A312-237A4E0B5FCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+      <selection activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4407,8 +4407,8 @@
       <c r="C183" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D183" s="4" t="s">
-        <v>4</v>
+      <c r="D183" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:4" ht="21">

</xml_diff>

<commit_message>
182. Find minimum swaps required to convert a Binary tree into BST
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4A13C2-04CC-4AB7-A312-237A4E0B5FCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7BC471-FE87-41F1-8FF2-C4A6DCE4FBC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D183" sqref="D183"/>
+      <selection activeCell="D187" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4463,8 +4463,8 @@
       <c r="C187" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="D187" s="4" t="s">
-        <v>4</v>
+      <c r="D187" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:4" ht="21">

</xml_diff>

<commit_message>
107. minimum no. of swaps required to sort the array
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7BC471-FE87-41F1-8FF2-C4A6DCE4FBC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94021E7F-374D-4763-B868-F06E7BE20E29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D187" sqref="D187"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3413,8 +3413,8 @@
       <c r="C112" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D112" s="4" t="s">
-        <v>4</v>
+      <c r="D112" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="21">

</xml_diff>

<commit_message>
90. Find first and last positions of an element in a sorted array
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94021E7F-374D-4763-B868-F06E7BE20E29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D82388-FFF9-4044-994B-89834E568A63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3175,8 +3175,8 @@
       <c r="C95" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>4</v>
+      <c r="D95" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="21">

</xml_diff>

<commit_message>
91. Find a Fixed Point (Value equal to index) in a given array
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D82388-FFF9-4044-994B-89834E568A63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEADBF5-0F04-4382-BB89-7ABCF0BBFA00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3189,8 +3189,8 @@
       <c r="C96" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>4</v>
+      <c r="D96" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="21">

</xml_diff>

<commit_message>
92. Search in a rotated sorted array
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEADBF5-0F04-4382-BB89-7ABCF0BBFA00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD51031E-9DF8-41B5-86A9-D97CD3B94E74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3203,8 +3203,8 @@
       <c r="C97" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D97" s="4" t="s">
-        <v>4</v>
+      <c r="D97" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="21">

</xml_diff>

<commit_message>
93. Square root of an integer
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD51031E-9DF8-41B5-86A9-D97CD3B94E74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40DAF1E-997F-429C-93AE-CDF0DE8B4093}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3217,8 +3217,8 @@
       <c r="C98" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D98" s="4" t="s">
-        <v>4</v>
+      <c r="D98" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="21">

</xml_diff>

<commit_message>
181. Construct Binary tree from Inorder and preorder traversal
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B372F5-CE20-42A0-9567-2A7C756F01B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF999CF4-612A-4F05-A0DA-A78B9878F80D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
+      <selection activeCell="D186" sqref="D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4449,8 +4449,8 @@
       <c r="C186" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D186" s="4" t="s">
-        <v>4</v>
+      <c r="D186" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:4" ht="21">

</xml_diff>

<commit_message>
183. Check if Binary tree is Sum tree or not
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF999CF4-612A-4F05-A0DA-A78B9878F80D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD0E415-7E9B-447B-BAF7-77C897F23C72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="D186" sqref="D186"/>
+      <selection activeCell="D188" sqref="D188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4477,8 +4477,8 @@
       <c r="C188" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="D188" s="4" t="s">
-        <v>4</v>
+      <c r="D188" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:4" ht="21">

</xml_diff>

<commit_message>
184. Check if all leaf nodes are at same level or not
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD0E415-7E9B-447B-BAF7-77C897F23C72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB46D7B7-D90D-4397-B635-85BD12BA6B2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="D188" sqref="D188"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4491,8 +4491,8 @@
       <c r="C189" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="D189" s="4" t="s">
-        <v>4</v>
+      <c r="D189" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:4" ht="21">

</xml_diff>

<commit_message>
185. Check if a Binary Tree contains duplicate subtrees of size 2 or more [ IMP ]
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB46D7B7-D90D-4397-B635-85BD12BA6B2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0250D0F3-7A1F-429D-8FA8-56F000857891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D189" sqref="D189"/>
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4505,8 +4505,8 @@
       <c r="C190" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D190" s="4" t="s">
-        <v>4</v>
+      <c r="D190" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="21">

</xml_diff>

<commit_message>
186. Check if 2 trees are mirror or not
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0250D0F3-7A1F-429D-8FA8-56F000857891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69D284-40E3-4204-B18F-59B2F8FA907C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+      <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4519,8 +4519,8 @@
       <c r="C191" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="D191" s="4" t="s">
-        <v>4</v>
+      <c r="D191" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="192" spans="1:4" ht="21">

</xml_diff>

<commit_message>
187. Sum of Nodes on the Longest path from root to leaf node
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD69D284-40E3-4204-B18F-59B2F8FA907C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB0FA5B-4B3E-4780-B71C-402ED97E7855}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191"/>
+      <selection activeCell="D192" sqref="D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4533,8 +4533,8 @@
       <c r="C192" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D192" s="4" t="s">
-        <v>4</v>
+      <c r="D192" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="21">

</xml_diff>

<commit_message>
189. Find Largest subtree sum in a tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB0FA5B-4B3E-4780-B71C-402ED97E7855}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A27A39-A212-48DF-8D53-521322812241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1882,7 +1882,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D192" sqref="D192"/>
+      <selection activeCell="D194" sqref="D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4547,8 +4547,8 @@
       <c r="C193" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D193" s="4" t="s">
-        <v>4</v>
+      <c r="D193" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="194" spans="1:4" ht="21">
@@ -4561,8 +4561,8 @@
       <c r="C194" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="D194" s="4" t="s">
-        <v>4</v>
+      <c r="D194" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="21">

</xml_diff>

<commit_message>
190. Maximum Sum of nodes in Binary tree such that no two are adjacent
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A27A39-A212-48DF-8D53-521322812241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD1F0B9-76FA-45C7-B872-096837576DBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1881,15 +1881,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="D194" sqref="D194"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="19.375" customWidth="1"/>
-    <col min="3" max="3" width="103.75" customWidth="1"/>
+    <col min="2" max="2" width="26.625" customWidth="1"/>
+    <col min="3" max="3" width="94.25" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4575,8 +4575,8 @@
       <c r="C195" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="D195" s="4" t="s">
-        <v>4</v>
+      <c r="D195" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="21">

</xml_diff>

<commit_message>
191. Print all K Sum paths in a Binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD1F0B9-76FA-45C7-B872-096837576DBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBB5774-9A42-437B-A565-085DC63207F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1531,7 +1531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1562,6 +1562,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1882,7 +1885,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="D195" sqref="D195"/>
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4589,8 +4592,8 @@
       <c r="C196" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="D196" s="4" t="s">
-        <v>4</v>
+      <c r="D196" s="14" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="197" spans="1:4" ht="21">
@@ -8641,5 +8644,6 @@
     <hyperlink ref="C2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId447"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
192. Find LCA in a Binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBB5774-9A42-437B-A565-085DC63207F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6805D0-C571-4BA3-B9E3-185041333E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1531,7 +1531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1565,6 +1565,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1885,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+      <selection activeCell="D200" sqref="D200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4606,8 +4609,8 @@
       <c r="C197" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>4</v>
+      <c r="D197" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="21">

</xml_diff>

<commit_message>
193. Find distance between 2 nodes in a Binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6805D0-C571-4BA3-B9E3-185041333E39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31842654-EDE7-419C-895B-D751EC3BFDB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="D200" sqref="D200"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4623,8 +4623,8 @@
       <c r="C198" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="D198" s="4" t="s">
-        <v>4</v>
+      <c r="D198" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="199" spans="1:4" ht="21">

</xml_diff>

<commit_message>
194. Kth Ancestor of node in a Binary tree
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31842654-EDE7-419C-895B-D751EC3BFDB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A98241D-3DF9-44DD-8ABC-39966BC3519B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="D198" sqref="D198"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="D199" sqref="D199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4637,8 +4637,8 @@
       <c r="C199" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="D199" s="4" t="s">
-        <v>4</v>
+      <c r="D199" s="15" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="21">

</xml_diff>

<commit_message>
197. Find a value in a BST
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A98241D-3DF9-44DD-8ABC-39966BC3519B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A8819C-E7A6-4A68-9705-82A60367C858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="D199" sqref="D199"/>
+      <selection activeCell="C202" sqref="C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4679,8 +4679,8 @@
       <c r="C202" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D202" s="4" t="s">
-        <v>4</v>
+      <c r="D202" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="203" spans="1:4" ht="21">

</xml_diff>

<commit_message>
126. Write a Program to reverse the Linked List. (Both Iterative and recursive)
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A8819C-E7A6-4A68-9705-82A60367C858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67613D70-A9DC-4716-9F91-A70043B0E135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="C202" sqref="C202"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3685,8 +3685,8 @@
       <c r="C131" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D131" s="4" t="s">
-        <v>4</v>
+      <c r="D131" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Reverse a Linked List in group of Given Size. [Very Imp]
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67613D70-A9DC-4716-9F91-A70043B0E135}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F72B476-3897-4D32-9212-7C7A1524454D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3699,8 +3699,8 @@
       <c r="C132" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D132" s="4" t="s">
-        <v>4</v>
+      <c r="D132" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="21">

</xml_diff>

<commit_message>
128. Write a program to Detect loop in a linked list.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F72B476-3897-4D32-9212-7C7A1524454D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96AFCBD-390F-4966-9515-1DE175994213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3713,8 +3713,8 @@
       <c r="C133" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D133" s="4" t="s">
-        <v>4</v>
+      <c r="D133" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="21">

</xml_diff>

<commit_message>
129. Write a program to Delete loop in a linked list.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96AFCBD-390F-4966-9515-1DE175994213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9242B085-D135-4342-B941-62E8491D4463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3727,8 +3727,8 @@
       <c r="C134" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D134" s="4" t="s">
-        <v>4</v>
+      <c r="D134" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="21">

</xml_diff>

<commit_message>
130. Find First Node of loop in a linked list
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9242B085-D135-4342-B941-62E8491D4463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A06C9-607D-4E45-B912-5F64CA03C992}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D134" sqref="D134"/>
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3741,8 +3741,8 @@
       <c r="C135" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="D135" s="4" t="s">
-        <v>4</v>
+      <c r="D135" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="21">

</xml_diff>

<commit_message>
131. Remove Duplicates in a sorted Linked List.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0A06C9-607D-4E45-B912-5F64CA03C992}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA616E51-0EC0-4D4D-B51E-322654F225BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3755,8 +3755,8 @@
       <c r="C136" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D136" s="4" t="s">
-        <v>4</v>
+      <c r="D136" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="21">

</xml_diff>

<commit_message>
132. Remove Duplicates in a Un-sorted Linked List.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA616E51-0EC0-4D4D-B51E-322654F225BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE23A8D6-3E2B-466F-A35F-0B51EAE53041}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D136" sqref="D136"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3769,8 +3769,8 @@
       <c r="C137" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D137" s="4" t="s">
-        <v>4</v>
+      <c r="D137" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="21">
@@ -4035,8 +4035,8 @@
       <c r="C156" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="D156" s="4" t="s">
-        <v>4</v>
+      <c r="D156" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="21">

</xml_diff>

<commit_message>
133. Write a Program to Move the last element to Front in a Linked List.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE23A8D6-3E2B-466F-A35F-0B51EAE53041}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A9E993-3338-44D4-9C70-A890873A97CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3783,8 +3783,8 @@
       <c r="C138" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D138" s="4" t="s">
-        <v>4</v>
+      <c r="D138" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="21">
@@ -4049,8 +4049,8 @@
       <c r="C157" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D157" s="4" t="s">
-        <v>4</v>
+      <c r="D157" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="21">

</xml_diff>

<commit_message>
134. Add 1 to a number represented as a Linked List.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A9E993-3338-44D4-9C70-A890873A97CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504719D7-F7D8-4003-9501-2DAB34FC3B4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C138" sqref="C138"/>
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3797,8 +3797,8 @@
       <c r="C139" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D139" s="4" t="s">
-        <v>4</v>
+      <c r="D139" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="21">

</xml_diff>

<commit_message>
135. Add two numbers represented by linked lists.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504719D7-F7D8-4003-9501-2DAB34FC3B4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABB4BDF-231C-4C90-B4B0-83B3547CD3FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3811,8 +3811,8 @@
       <c r="C140" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D140" s="4" t="s">
-        <v>4</v>
+      <c r="D140" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="21">

</xml_diff>

<commit_message>
136. Intersection of two Sorted Linked List.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABB4BDF-231C-4C90-B4B0-83B3547CD3FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4C0498-300D-400C-B19E-E7E01910D242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+      <selection activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3825,8 +3825,8 @@
       <c r="C141" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D141" s="4" t="s">
-        <v>4</v>
+      <c r="D141" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="21">

</xml_diff>

<commit_message>
137. Intersection Point of two Linked Lists.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4C0498-300D-400C-B19E-E7E01910D242}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCB0D21-F3E9-42CA-AC53-470F1510AC60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D141" sqref="D141"/>
+      <selection activeCell="D142" sqref="D142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3839,8 +3839,8 @@
       <c r="C142" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D142" s="4" t="s">
-        <v>4</v>
+      <c r="D142" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="21">

</xml_diff>

<commit_message>
140 .Find the middle Element of a linked list.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCB0D21-F3E9-42CA-AC53-470F1510AC60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ACB84B-4ACA-4A25-8749-9941FFFB09DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
138. Merge Sort For Linked lists.[Very Important]
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8ACB84B-4ACA-4A25-8749-9941FFFB09DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D80774-0CDD-4E21-912D-49C9C0BE2E51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3853,8 +3853,8 @@
       <c r="C143" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D143" s="4" t="s">
-        <v>4</v>
+      <c r="D143" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="21">
@@ -3881,8 +3881,8 @@
       <c r="C145" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="D145" s="4" t="s">
-        <v>4</v>
+      <c r="D145" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="21">

</xml_diff>

<commit_message>
141. Check If Circular Linked List
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D80774-0CDD-4E21-912D-49C9C0BE2E51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA0D66B-9C85-4C89-8B81-104B2E8B15F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3867,8 +3867,8 @@
       <c r="C144" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="D144" s="4" t="s">
-        <v>4</v>
+      <c r="D144" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="21">
@@ -3895,8 +3895,8 @@
       <c r="C146" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D146" s="4" t="s">
-        <v>4</v>
+      <c r="D146" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="21">

</xml_diff>

<commit_message>
142. Split a Circular linked list into two halves.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA0D66B-9C85-4C89-8B81-104B2E8B15F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E12512-12EE-4B84-9688-E4A568CF0977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="C147" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3909,8 +3909,8 @@
       <c r="C147" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D147" s="4" t="s">
-        <v>4</v>
+      <c r="D147" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="21">

</xml_diff>

<commit_message>
143. Write a Program to check whether the Singly Linked list is a palindrome or not.
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E12512-12EE-4B84-9688-E4A568CF0977}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B2872-9A08-4048-B9F7-B26A6B05FBFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1888,7 +1888,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+      <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3923,8 +3923,8 @@
       <c r="C148" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D148" s="4" t="s">
-        <v>4</v>
+      <c r="D148" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="21">

</xml_diff>

<commit_message>
159. Segregate even and odd nodes in a Linked List
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876B2872-9A08-4048-B9F7-B26A6B05FBFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A29481-59A7-4A68-B2DE-66DC64C35DB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1887,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3937,8 +3937,8 @@
       <c r="C149" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="D149" s="4" t="s">
-        <v>4</v>
+      <c r="D149" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="21">
@@ -4147,8 +4147,8 @@
       <c r="C164" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="D164" s="4" t="s">
-        <v>4</v>
+      <c r="D164" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="21">

</xml_diff>

<commit_message>
335. Implement DFS Algorithm.cpp
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding\CP-Solving-Streak - GITHUB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive - KLK VENTURES PRIVATE LIMITED\Desktop\CP-Solving-Streak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A29481-59A7-4A68-B2DE-66DC64C35DB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1428,7 +1427,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -1884,22 +1883,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+    <sheetView tabSelected="1" topLeftCell="B330" workbookViewId="0">
+      <selection activeCell="D336" sqref="D336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="26.625" customWidth="1"/>
+    <col min="2" max="2" width="26.58203125" customWidth="1"/>
     <col min="3" max="3" width="94.25" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.25">
+    <row r="1" spans="1:4" ht="25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6527,8 +6526,8 @@
       <c r="C334" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="D334" s="4" t="s">
-        <v>4</v>
+      <c r="D334" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="335" spans="1:4" ht="21">
@@ -6541,8 +6540,8 @@
       <c r="C335" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="D335" s="4" t="s">
-        <v>4</v>
+      <c r="D335" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="336" spans="1:4" ht="21">
@@ -6555,8 +6554,8 @@
       <c r="C336" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="D336" s="4" t="s">
-        <v>4</v>
+      <c r="D336" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="337" spans="1:4" ht="21">
@@ -8199,452 +8198,452 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{2D6F1134-3C08-7445-B19A-9B94A18B55C7}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{E5A98931-37E8-6B4A-90BE-8DC72405341A}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{02736918-E09F-7A46-90B3-AFCC33AA559B}"/>
-    <hyperlink ref="C10" r:id="rId5" xr:uid="{6E8DD30A-A9F9-4C44-B26C-C9E236F10798}"/>
-    <hyperlink ref="C11" r:id="rId6" xr:uid="{0D55765B-95A7-154F-96F3-B7E4C581021F}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{6F687ABA-C04B-AF4F-9F11-A038DCB20FB9}"/>
-    <hyperlink ref="C13" r:id="rId8" xr:uid="{11C9D8CC-9F1E-004E-8EC2-C758DC9C8CAB}"/>
-    <hyperlink ref="C14" r:id="rId9" xr:uid="{56E4962F-CB3D-9E48-A26E-19A1F5C800C9}"/>
-    <hyperlink ref="C15" r:id="rId10" xr:uid="{899DDBD9-9ED6-3A4D-8AFE-8FAA6DA88DBC}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{76D41EAC-A28A-2845-8515-CA3C70D823B7}"/>
-    <hyperlink ref="C17" r:id="rId12" xr:uid="{828948BE-DD97-DE4A-BAD6-B415E29198F0}"/>
-    <hyperlink ref="C18" r:id="rId13" xr:uid="{E98C86AA-12E7-124C-B7D0-BCDFB246040B}"/>
-    <hyperlink ref="C19" r:id="rId14" xr:uid="{192741A9-FF68-DC4A-99FA-69F9968AB4F2}"/>
-    <hyperlink ref="C20" r:id="rId15" xr:uid="{DBD9BA9C-91C6-B144-A800-DCB3BED33DE7}"/>
-    <hyperlink ref="C21" r:id="rId16" xr:uid="{A285BDE8-00E7-A94C-8E43-A0C4829D42FA}"/>
-    <hyperlink ref="C22" r:id="rId17" xr:uid="{B0C21764-2962-1649-8AFA-10FB9420C5FC}"/>
-    <hyperlink ref="C23" r:id="rId18" xr:uid="{9282CC15-9B38-E54B-B64C-557745C9C00A}"/>
-    <hyperlink ref="C24" r:id="rId19" xr:uid="{3BCCEBE2-AC3B-AC4F-8BA9-439ACEA133D4}"/>
-    <hyperlink ref="C25" r:id="rId20" xr:uid="{74F8D761-6EBF-594A-A6C7-40DE4CE96958}"/>
-    <hyperlink ref="C26" r:id="rId21" xr:uid="{79947FE6-D417-D644-81D8-D058180550A0}"/>
-    <hyperlink ref="C27" r:id="rId22" xr:uid="{2BF3F606-410B-264D-BF60-191C34D616BB}"/>
-    <hyperlink ref="C28" r:id="rId23" xr:uid="{CD98DB26-0F2F-FD40-A989-53FE548D7D34}"/>
-    <hyperlink ref="C29" r:id="rId24" xr:uid="{307032A1-F8EF-1A48-BFE3-EA3283D39BE2}"/>
-    <hyperlink ref="C30" r:id="rId25" xr:uid="{AA329F36-941A-9241-9402-9D220B05E719}"/>
-    <hyperlink ref="C31" r:id="rId26" xr:uid="{9E851DAC-0E30-B340-84F9-721D70B66919}"/>
-    <hyperlink ref="C32" r:id="rId27" xr:uid="{468380BA-4978-A645-ABD0-E74FD3E6BDBB}"/>
-    <hyperlink ref="C33" r:id="rId28" xr:uid="{289E6890-8CCB-D645-9B3F-6138FFC1C249}"/>
-    <hyperlink ref="C34" r:id="rId29" xr:uid="{8EABDC68-858F-784A-A8F1-C603E3B8C1FE}"/>
-    <hyperlink ref="C35" r:id="rId30" xr:uid="{6157E427-1210-3F45-A4DC-6DFD2373B9CF}"/>
-    <hyperlink ref="C36" r:id="rId31" xr:uid="{2D7BA55E-9947-FF4D-BC09-FB4A5ADA07EC}"/>
-    <hyperlink ref="C37" r:id="rId32" xr:uid="{3337C74F-8B73-E64E-A6DA-5D9F7C7B4D32}"/>
-    <hyperlink ref="C38" r:id="rId33" xr:uid="{02370124-E58D-B540-BBCF-98266229556D}"/>
-    <hyperlink ref="C39" r:id="rId34" xr:uid="{F2DE2162-BD02-7549-AC1A-27455F78131F}"/>
-    <hyperlink ref="C40" r:id="rId35" xr:uid="{6FA286B9-3994-624D-B0B8-C01657D110AD}"/>
-    <hyperlink ref="C41" r:id="rId36" xr:uid="{6EFBEDA1-5C10-2547-8FB2-44E977513B28}"/>
-    <hyperlink ref="C42" r:id="rId37" xr:uid="{090EC515-BEBE-514E-BA59-A84E450B4211}"/>
-    <hyperlink ref="C43" r:id="rId38" xr:uid="{0A0557FD-77E5-564B-B100-147D544A38B4}"/>
-    <hyperlink ref="C44" r:id="rId39" xr:uid="{3F82F2E0-AA59-5042-B079-F3B3C6FF2FD7}"/>
-    <hyperlink ref="C45" r:id="rId40" xr:uid="{FFF7D257-1F58-5A4B-AAA2-F5480AED86C7}"/>
-    <hyperlink ref="C46" r:id="rId41" xr:uid="{353E28FA-E36D-7447-9DE8-787DF11C4669}"/>
-    <hyperlink ref="C47" r:id="rId42" xr:uid="{F9B53127-FC98-FE43-B53F-BFDBCE2A4427}"/>
-    <hyperlink ref="C48" r:id="rId43" xr:uid="{40685BBC-CE24-624E-9ABB-98490B7DE0E4}"/>
-    <hyperlink ref="C49" r:id="rId44" xr:uid="{7733D505-2EC7-E346-B3DA-C980C7CE0B27}"/>
-    <hyperlink ref="C50" r:id="rId45" xr:uid="{E8C1FE00-7B4B-5745-8E4B-CD44B6C749E3}"/>
-    <hyperlink ref="C51" r:id="rId46" xr:uid="{FDE181B1-57B0-7C4B-A189-C7C6E4EAEF99}"/>
-    <hyperlink ref="C52" r:id="rId47" xr:uid="{FE85FD72-4FC9-334E-8205-9E8B238954EB}"/>
-    <hyperlink ref="C53" r:id="rId48" xr:uid="{7630AD76-7E6B-8C4A-BA33-A62EBB042215}"/>
-    <hyperlink ref="C54" r:id="rId49" xr:uid="{2A738B70-CBF0-CC40-8B05-A271822B3F1A}"/>
-    <hyperlink ref="C56" r:id="rId50" xr:uid="{B2DE2D9E-8371-CD44-9D0D-4D6DC64AC29B}"/>
-    <hyperlink ref="C57" r:id="rId51" xr:uid="{265DCD11-17A0-654E-BEFE-FABA31210C6E}"/>
-    <hyperlink ref="C58" r:id="rId52" xr:uid="{47F1BB0C-0C5C-0845-8EEC-1560C50D7DA7}"/>
-    <hyperlink ref="C59" r:id="rId53" xr:uid="{8E0BFA2E-CCB4-514F-86CD-78176C6CC98A}"/>
-    <hyperlink ref="C60" r:id="rId54" xr:uid="{E4DEFB4B-749F-8746-97C7-F2B433664A74}"/>
-    <hyperlink ref="C61" r:id="rId55" xr:uid="{8301BDBD-EB7E-7D41-A777-ED99C3F9D67D}"/>
-    <hyperlink ref="C62" r:id="rId56" xr:uid="{927AE532-647F-AF4C-A567-40ADA6FCE534}"/>
-    <hyperlink ref="C63" r:id="rId57" xr:uid="{05489F52-CC92-EC44-9AD3-773DEC3B1D36}"/>
-    <hyperlink ref="C64" r:id="rId58" xr:uid="{13025DF6-C30E-014A-B66C-68C4AAAC1C6E}"/>
-    <hyperlink ref="C65" r:id="rId59" xr:uid="{BEE1F613-C189-B949-A225-0E0C5AFD1532}"/>
-    <hyperlink ref="C66" r:id="rId60" xr:uid="{1DFECD6C-D7CC-0340-B29B-4D56E50711E5}"/>
-    <hyperlink ref="C67" r:id="rId61" xr:uid="{70BED156-B004-E043-BF7D-59EFAA9EADAF}"/>
-    <hyperlink ref="C68" r:id="rId62" xr:uid="{FF9CBAFB-900E-E242-8B33-EDF46F0F40B5}"/>
-    <hyperlink ref="C69" r:id="rId63" xr:uid="{19461114-B3E8-9042-8029-100010946A04}"/>
-    <hyperlink ref="C70" r:id="rId64" xr:uid="{00F71118-E30B-A84E-819E-FFA902C70502}"/>
-    <hyperlink ref="C71" r:id="rId65" xr:uid="{58E70966-BBE0-7743-A250-AE4DD57807DE}"/>
-    <hyperlink ref="C72" r:id="rId66" xr:uid="{09409FE3-9D7E-4F43-BB21-14A1B8D6E480}"/>
-    <hyperlink ref="C73" r:id="rId67" xr:uid="{E199A3DC-3DA1-C648-93C0-DF9CD5331204}"/>
-    <hyperlink ref="C74" r:id="rId68" xr:uid="{85886847-1510-AA46-B10C-F3D80591DD74}"/>
-    <hyperlink ref="C75" r:id="rId69" xr:uid="{F60808FC-F09D-FC44-B2DD-752E55A1C698}"/>
-    <hyperlink ref="C76" r:id="rId70" xr:uid="{16B2725E-1AD5-0441-9B5B-B6B2F458091B}"/>
-    <hyperlink ref="C77" r:id="rId71" xr:uid="{8440D753-5DE9-3243-97C2-C09D195C325F}"/>
-    <hyperlink ref="C78" r:id="rId72" xr:uid="{AC63A963-B6CC-6E4E-B72A-7F472BC4C027}"/>
-    <hyperlink ref="C79" r:id="rId73" xr:uid="{B21B87F1-A0C0-7F4E-B36F-912B871D0EF4}"/>
-    <hyperlink ref="C80" r:id="rId74" xr:uid="{789FFFAC-8B7E-0540-98B8-856430EB56F8}"/>
-    <hyperlink ref="C81" r:id="rId75" xr:uid="{4A0E959E-22F4-6948-A819-76FE76AB9F6D}"/>
-    <hyperlink ref="C82" r:id="rId76" xr:uid="{78B76678-D8EE-9745-98B1-DF7A76EA3B10}"/>
-    <hyperlink ref="C83" r:id="rId77" xr:uid="{62982242-1D19-1544-8653-8E25E9BF4505}"/>
-    <hyperlink ref="C84" r:id="rId78" xr:uid="{8E3D4BDF-9F8F-0542-BFD8-C3CE3BF396E6}"/>
-    <hyperlink ref="C85" r:id="rId79" xr:uid="{A3D51762-65A1-9A44-B619-D1D98A7F403B}"/>
-    <hyperlink ref="C86" r:id="rId80" xr:uid="{ED0F5FC7-0066-EB44-8FCF-460600DADB02}"/>
-    <hyperlink ref="C87" r:id="rId81" xr:uid="{2D956AC4-4774-7446-8473-C4CE00E33C17}"/>
-    <hyperlink ref="C88" r:id="rId82" xr:uid="{C8C607BB-1FEE-FA47-9E3E-6C0BCE978B7F}"/>
-    <hyperlink ref="C89" r:id="rId83" xr:uid="{B9AC5194-6D36-684A-A5C4-BEE11037599F}"/>
-    <hyperlink ref="C90" r:id="rId84" xr:uid="{AB28D9E6-890C-F14A-A5FB-2303BE319968}"/>
-    <hyperlink ref="C91" r:id="rId85" xr:uid="{1F507CBC-4056-AD46-9314-95ECBB9D799D}"/>
-    <hyperlink ref="C92" r:id="rId86" xr:uid="{F152A9AF-5CBA-EC44-A9CF-07AB481435AB}"/>
-    <hyperlink ref="C93" r:id="rId87" xr:uid="{346CA74F-60B7-0A4B-A612-9184D4DCFF62}"/>
-    <hyperlink ref="C94" r:id="rId88" xr:uid="{8C653CB1-4954-754F-8D46-F09141A2FCDB}"/>
-    <hyperlink ref="C95" r:id="rId89" xr:uid="{5989F693-2A61-A346-8395-8674307A4CC2}"/>
-    <hyperlink ref="C96" r:id="rId90" xr:uid="{3AD10C9E-4F6D-DE48-92F3-531A586520C6}"/>
-    <hyperlink ref="C97" r:id="rId91" xr:uid="{4FA217C0-A1F3-904E-8FEA-EA4941273A67}"/>
-    <hyperlink ref="C98" r:id="rId92" xr:uid="{A297BBC0-FA0D-2D46-9C49-3932193EF1D3}"/>
-    <hyperlink ref="C100" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance." xr:uid="{DCD751DE-E440-F346-B6FD-CBD072217214}"/>
-    <hyperlink ref="C101" r:id="rId94" xr:uid="{B2FD38B9-1E2B-8140-8291-F45734C98145}"/>
-    <hyperlink ref="C102" r:id="rId95" xr:uid="{C76888B3-18AC-9B48-9E2A-64A7DF0902B7}"/>
-    <hyperlink ref="C103" r:id="rId96" xr:uid="{18A79860-6C9E-A941-8D6C-360B9913E941}"/>
-    <hyperlink ref="C104" r:id="rId97" xr:uid="{C0DDFD68-CBC1-0F4A-AF40-ACF36BBC8453}"/>
-    <hyperlink ref="C105" r:id="rId98" xr:uid="{3E0BF737-E42E-C946-B32C-06882E0BA6FF}"/>
-    <hyperlink ref="C107" r:id="rId99" xr:uid="{862F9782-C57B-2848-A2D9-EB7B52FB7EC7}"/>
-    <hyperlink ref="C108" r:id="rId100" xr:uid="{230D7A6A-D2C5-C140-9A65-B1F407D22062}"/>
-    <hyperlink ref="C109" r:id="rId101" xr:uid="{BDC2BA28-4562-984E-8282-1126BF952EAF}"/>
-    <hyperlink ref="C110" r:id="rId102" xr:uid="{B53A5F28-6DED-3D47-8679-F78D3DDEFF01}"/>
-    <hyperlink ref="C111" r:id="rId103" xr:uid="{C57D0CC7-DA2F-0948-9BCE-F19C20C7D981}"/>
-    <hyperlink ref="C112" r:id="rId104" xr:uid="{117878E5-B8C8-254B-8ED6-014B4B7A8126}"/>
-    <hyperlink ref="C113" r:id="rId105" xr:uid="{B7CC0756-74F2-D54D-BDEE-9DA394DD7168}"/>
-    <hyperlink ref="C114" r:id="rId106" xr:uid="{837EF472-CCC2-CF47-A8A8-238E56F722CE}"/>
-    <hyperlink ref="C115" r:id="rId107" xr:uid="{3608F267-6AA0-624B-B243-7DDD317E9F08}"/>
-    <hyperlink ref="C116" r:id="rId108" xr:uid="{0B6123E6-0472-374B-ACA7-6914CD7918E8}"/>
-    <hyperlink ref="C117" r:id="rId109" xr:uid="{D3971CEB-C53E-B04B-9C32-1803182B5DC5}"/>
-    <hyperlink ref="C118" r:id="rId110" xr:uid="{7CF5013A-643E-1643-93A1-A2F1500D2A23}"/>
-    <hyperlink ref="C119" r:id="rId111" xr:uid="{2A6BE7E5-D818-6843-8C3E-99EA2BFE0FB2}"/>
-    <hyperlink ref="C120" r:id="rId112" xr:uid="{E718F544-96DF-A04E-8DFB-7639DA3EA57C}"/>
-    <hyperlink ref="C121" r:id="rId113" xr:uid="{B0C2F065-424A-7345-A864-346ECD98D749}"/>
-    <hyperlink ref="C122" r:id="rId114" xr:uid="{B4E26955-5C3F-804E-B19A-11260310AFB3}"/>
-    <hyperlink ref="C123" r:id="rId115" xr:uid="{6F299BB5-8E82-0240-A9A3-6829CE3ABCBF}"/>
-    <hyperlink ref="C124" r:id="rId116" xr:uid="{A42CA32F-2196-1840-A53D-E5073237C68D}"/>
-    <hyperlink ref="C125" r:id="rId117" xr:uid="{7ECF6EF4-962E-4642-9B1C-C3B70674793E}"/>
-    <hyperlink ref="C126" r:id="rId118" xr:uid="{2A109178-6B60-164E-9D25-42B3282137E3}"/>
-    <hyperlink ref="C127" r:id="rId119" xr:uid="{B3D38BD0-A6A1-8D41-8405-45E1BEEEEF06}"/>
-    <hyperlink ref="C128" r:id="rId120" xr:uid="{A1C26612-D040-2A41-A6A6-A8F2490C0A43}"/>
-    <hyperlink ref="C129" r:id="rId121" xr:uid="{C476E807-64CB-F44A-A23D-D21EBF6D001D}"/>
-    <hyperlink ref="C130" r:id="rId122" xr:uid="{9A414D55-D4A1-F147-9207-61B597D57136}"/>
-    <hyperlink ref="C99" r:id="rId123" xr:uid="{18B028A7-9B6F-D841-8548-924D70530779}"/>
-    <hyperlink ref="C106" r:id="rId124" xr:uid="{6D3E75EF-733F-7A4B-81C8-AEF6CB6335F0}"/>
-    <hyperlink ref="C131" r:id="rId125" xr:uid="{C9EB2682-BE0B-934B-B0B4-1DD1A1502647}"/>
-    <hyperlink ref="C132" r:id="rId126" xr:uid="{2992FED9-2B78-A342-92AA-E7C0F882FF17}"/>
-    <hyperlink ref="C133" r:id="rId127" xr:uid="{0084DA6F-EC84-BD48-BDA8-EBACA3BB3B3E}"/>
-    <hyperlink ref="C134" r:id="rId128" xr:uid="{30F2D415-4B2C-384C-8EAE-2CC71CB518E2}"/>
-    <hyperlink ref="C135" r:id="rId129" xr:uid="{40734C88-7C5B-9747-86D1-03463D9AD41A}"/>
-    <hyperlink ref="C136" r:id="rId130" xr:uid="{1040D22F-6729-104A-A229-CBDCED93024A}"/>
-    <hyperlink ref="C137" r:id="rId131" xr:uid="{E131FE61-FABF-8E4B-8EF0-F68379D8F836}"/>
-    <hyperlink ref="C138" r:id="rId132" xr:uid="{B2129272-1351-3745-883B-E6A7115450C8}"/>
-    <hyperlink ref="C139" r:id="rId133" xr:uid="{C8B2DEF0-2B69-C84E-8013-0B6F03FFC250}"/>
-    <hyperlink ref="C140" r:id="rId134" xr:uid="{536AC5CF-712F-BF48-94A9-D0E7DC013020}"/>
-    <hyperlink ref="C141" r:id="rId135" xr:uid="{2DABC9C7-43D4-1249-AF9B-5FA4552611CB}"/>
-    <hyperlink ref="C142" r:id="rId136" xr:uid="{DA62E73A-B495-F94A-BECE-D42E4CBF074A}"/>
-    <hyperlink ref="C143" r:id="rId137" xr:uid="{7F5E6966-850D-4F49-B2A5-678365713F28}"/>
-    <hyperlink ref="C144" r:id="rId138" xr:uid="{E9C4286D-8493-9A47-8B8C-09583FA72B70}"/>
-    <hyperlink ref="C145" r:id="rId139" xr:uid="{9EB0123C-84AE-1C4D-BA1A-C28CFB8EFB89}"/>
-    <hyperlink ref="C146" r:id="rId140" xr:uid="{9D11FED4-328F-674E-889D-EC781DD1D791}"/>
-    <hyperlink ref="C147" r:id="rId141" xr:uid="{48AE72DB-397B-464D-88AD-B8058ED29CC1}"/>
-    <hyperlink ref="C148" r:id="rId142" xr:uid="{152D50E9-7448-F542-AC66-05D0AE66664C}"/>
-    <hyperlink ref="C149" r:id="rId143" xr:uid="{34E6AF1B-5FB1-3A4B-8938-1DCF80831DC2}"/>
-    <hyperlink ref="C150" r:id="rId144" xr:uid="{E7F8B7CA-49F4-1946-91EE-E7582BE4E5DA}"/>
-    <hyperlink ref="C151" r:id="rId145" xr:uid="{3590A994-B7A2-C14D-9BF8-7AC8FE9E7F0F}"/>
-    <hyperlink ref="C152" r:id="rId146" xr:uid="{0AAA4B0C-4921-C34D-B41E-D702FA860892}"/>
-    <hyperlink ref="C153" r:id="rId147" xr:uid="{5973FCA4-AE32-5248-A6ED-2694367332F1}"/>
-    <hyperlink ref="C154" r:id="rId148" xr:uid="{4C0F816E-F043-0C47-BF16-1CDAD88D2FF1}"/>
-    <hyperlink ref="C155" r:id="rId149" xr:uid="{A8E4C654-D0BD-8945-9F5C-B09F7BC114BE}"/>
-    <hyperlink ref="C158" r:id="rId150" xr:uid="{E3825C15-10BB-E24F-B229-983F651DA942}"/>
-    <hyperlink ref="C159" r:id="rId151" xr:uid="{46ECFC31-388C-6241-8FFE-DED6F2FC794A}"/>
-    <hyperlink ref="C160" r:id="rId152" xr:uid="{589E024D-3FE1-1048-890C-88289733F233}"/>
-    <hyperlink ref="C161" r:id="rId153" xr:uid="{CDA28F7A-7FC5-F74D-B27E-A6E0161D41D5}"/>
-    <hyperlink ref="C162" r:id="rId154" xr:uid="{DA6A0D92-DCEB-DA4F-8BBA-10FCD092838F}"/>
-    <hyperlink ref="C163" r:id="rId155" xr:uid="{955769DB-3256-254B-90DE-E1E01B272F8A}"/>
-    <hyperlink ref="C164" r:id="rId156" xr:uid="{DED7AC9B-40D7-0545-9D6F-6CD4F5FFE4C6}"/>
-    <hyperlink ref="C165" r:id="rId157" xr:uid="{6947A4E1-B6AA-6D4F-A6D8-8FA74FD02887}"/>
-    <hyperlink ref="C166" r:id="rId158" xr:uid="{EABF2012-5A90-0C4E-86F6-FDB5FA7770BE}"/>
-    <hyperlink ref="C167" r:id="rId159" xr:uid="{7F44CFE0-9ED1-A44D-B9EF-CF87BEB644FC}"/>
-    <hyperlink ref="C168" r:id="rId160" xr:uid="{CF6E0CF6-7A93-D84A-9CE0-5BDD51767416}"/>
-    <hyperlink ref="C169" r:id="rId161" xr:uid="{EFF8F154-60B8-B84B-84CA-32756BD6430F}"/>
-    <hyperlink ref="C170" r:id="rId162" xr:uid="{C8A3094E-E11B-2543-B05E-1D07048B2EBA}"/>
-    <hyperlink ref="C171" r:id="rId163" xr:uid="{9961E5F5-B5C6-0C4D-A1D0-D04D2A5D7DFD}"/>
-    <hyperlink ref="C172" r:id="rId164" xr:uid="{44E289EC-47DD-D94D-88C1-CB2F59C6C16A}"/>
-    <hyperlink ref="C173" r:id="rId165" xr:uid="{4161FC70-DD6D-684B-898A-A4711596B2D5}"/>
-    <hyperlink ref="C174" r:id="rId166" xr:uid="{B9CBE387-8E9A-ED48-8310-CF7D34FA690C}"/>
-    <hyperlink ref="C175" r:id="rId167" xr:uid="{5398097B-24FF-9543-8F02-33CE2860F1F7}"/>
-    <hyperlink ref="C176" r:id="rId168" xr:uid="{3B1FC30B-30C8-7B48-AF94-A81FB513F24F}"/>
-    <hyperlink ref="C177" r:id="rId169" xr:uid="{32B750D0-D7F2-694D-AB9B-25AFAFAFF17F}"/>
-    <hyperlink ref="C178" r:id="rId170" xr:uid="{400689DD-8E95-024E-976B-AACD8ED4E1A6}"/>
-    <hyperlink ref="C179" r:id="rId171" xr:uid="{28753DDE-E047-5D40-A30B-1103BE6DA08F}"/>
-    <hyperlink ref="C180" r:id="rId172" xr:uid="{6C5AA6CB-3D93-0740-AEED-9E6C218CF6CB}"/>
-    <hyperlink ref="C181" r:id="rId173" xr:uid="{03EAA2B9-D8B8-D642-BF24-380596D26B2E}"/>
-    <hyperlink ref="C182" r:id="rId174" xr:uid="{8C1719B4-37CC-484E-BDCE-A4272C07F91B}"/>
-    <hyperlink ref="C183" r:id="rId175" xr:uid="{6C198DA2-BB98-F940-8EF6-2FC8B7AE577A}"/>
-    <hyperlink ref="C184" r:id="rId176" xr:uid="{AB0EA311-A446-D046-A0EC-290B42068328}"/>
-    <hyperlink ref="C185" r:id="rId177" xr:uid="{DB913045-B9F6-6549-AA09-22B0CC5FDD21}"/>
-    <hyperlink ref="C186" r:id="rId178" xr:uid="{806469FD-617A-7445-AAB5-FB2FD2ED24EA}"/>
-    <hyperlink ref="C187" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010." xr:uid="{1A10544E-58CF-D04D-9FAF-2FEC6DB2B5D4}"/>
-    <hyperlink ref="C188" r:id="rId180" xr:uid="{5A0B6645-89FD-E044-A706-9FB890274C3C}"/>
-    <hyperlink ref="C189" r:id="rId181" xr:uid="{B42A3009-E8EB-EE44-885F-6699C17A0E0B}"/>
-    <hyperlink ref="C190" r:id="rId182" xr:uid="{ED3E48AB-E25B-3744-B024-E97B2A319B46}"/>
-    <hyperlink ref="C191" r:id="rId183" xr:uid="{C75D20A3-CBAE-2649-A3EE-E49177CFA343}"/>
-    <hyperlink ref="C192" r:id="rId184" xr:uid="{3863CA1B-D43E-1144-91A9-17C2DCF52A64}"/>
-    <hyperlink ref="C193" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not." xr:uid="{E9AF434E-4CAA-5D49-8AD3-889CDE2913D9}"/>
-    <hyperlink ref="C194" r:id="rId186" xr:uid="{1A0568E5-3A11-7F47-8001-82B05D7C2339}"/>
-    <hyperlink ref="C195" r:id="rId187" xr:uid="{F62B8AE4-9C4F-9544-8861-CD733C12F79E}"/>
-    <hyperlink ref="C196" r:id="rId188" xr:uid="{0F6A542C-44C9-5A4C-90BF-BC8C239877D2}"/>
-    <hyperlink ref="C197" r:id="rId189" xr:uid="{3ED28203-B1B5-4E46-AAF3-779EDD4AC03F}"/>
-    <hyperlink ref="C198" r:id="rId190" xr:uid="{4338B305-B52F-5540-9B51-B938FC6803A2}"/>
-    <hyperlink ref="C199" r:id="rId191" xr:uid="{DDEEED0F-A939-1E4F-B2FA-AD391A4A2874}"/>
-    <hyperlink ref="C200" r:id="rId192" xr:uid="{C2F20589-AD81-654C-94E5-E5B6C9FE27F6}"/>
-    <hyperlink ref="C201" r:id="rId193" xr:uid="{BBEB9DAC-E4AE-C04F-AA15-6356AFC57FDE}"/>
-    <hyperlink ref="C202" r:id="rId194" xr:uid="{6316566D-A10A-F849-9F25-B9ED4DA12BC7}"/>
-    <hyperlink ref="C203" r:id="rId195" xr:uid="{9D4DD895-FBA6-C849-A5BF-3B30755BD9C9}"/>
-    <hyperlink ref="C204" r:id="rId196" xr:uid="{475996DA-632A-BE49-AEA1-D4189FD614A1}"/>
-    <hyperlink ref="C205" r:id="rId197" xr:uid="{88E0C858-8468-884F-BB71-F6F176BD5FC2}"/>
-    <hyperlink ref="C206" r:id="rId198" xr:uid="{C1C5C8D0-7A06-3D4A-A85A-AAACC1B418C9}"/>
-    <hyperlink ref="C207" r:id="rId199" xr:uid="{D525D4B1-2857-1543-8CD9-196728321203}"/>
-    <hyperlink ref="C208" r:id="rId200" xr:uid="{51E3AB9B-04B2-C041-A2B3-37E3EB18013A}"/>
-    <hyperlink ref="C209" r:id="rId201" xr:uid="{7F7F0C9A-57B9-314F-959A-B8ACAFA5FD13}"/>
-    <hyperlink ref="C210" r:id="rId202" xr:uid="{3B029785-83B4-6140-8B70-CD892CFC87F6}"/>
-    <hyperlink ref="C211" r:id="rId203" xr:uid="{B0A390E6-D860-9F4E-B021-68949FE712F3}"/>
-    <hyperlink ref="C212" r:id="rId204" xr:uid="{49E9953D-52F6-BF47-8AAA-8E456F55576B}"/>
-    <hyperlink ref="C213" r:id="rId205" xr:uid="{9B812470-F419-A54E-8365-06A9B8864A30}"/>
-    <hyperlink ref="C214" r:id="rId206" xr:uid="{B6FB4107-1933-6D45-9EF4-4474E06CBE9D}"/>
-    <hyperlink ref="C215" r:id="rId207" xr:uid="{0F7C1D92-7BCB-D14D-A658-9599984E04E4}"/>
-    <hyperlink ref="C216" r:id="rId208" xr:uid="{6810428F-0A78-964C-A8C8-E1CD2E7C405D}"/>
-    <hyperlink ref="C217" r:id="rId209" xr:uid="{B40209F2-0D6E-364F-8AF6-F1D182509314}"/>
-    <hyperlink ref="C218" r:id="rId210" xr:uid="{96C53FA9-9FD3-2D4F-B292-3C9DEDFA806E}"/>
-    <hyperlink ref="C219" r:id="rId211" xr:uid="{918B420D-3678-FD46-9463-595E8ACC39E1}"/>
-    <hyperlink ref="C220" r:id="rId212" xr:uid="{851A7153-3B54-0E4A-A0A0-FCEB091AFE70}"/>
-    <hyperlink ref="C221" r:id="rId213" xr:uid="{C03AE9F8-09AE-C640-81A7-033BB06FB6AD}"/>
-    <hyperlink ref="C222" r:id="rId214" xr:uid="{35140DEB-52D2-4342-88D2-22BA061E5B48}"/>
-    <hyperlink ref="C223" r:id="rId215" xr:uid="{9714BC0B-3373-934C-B7A1-599F74F4FB9D}"/>
-    <hyperlink ref="C224" r:id="rId216" xr:uid="{5CB435B2-7FD2-1D44-9872-22B6A1EDC02B}"/>
-    <hyperlink ref="C225" r:id="rId217" xr:uid="{722D1D95-896B-4642-BABD-31DEDD237B49}"/>
-    <hyperlink ref="C226" r:id="rId218" xr:uid="{D686D1DC-13D6-284C-B606-E087FAF47399}"/>
-    <hyperlink ref="C227" r:id="rId219" xr:uid="{D22C2394-C3CB-8F4F-A010-2B13C8C84D1A}"/>
-    <hyperlink ref="C228" r:id="rId220" xr:uid="{3AE2F800-B66F-1A41-893B-978F6875FDC8}"/>
-    <hyperlink ref="C229" r:id="rId221" xr:uid="{2C939BDE-5298-5541-837B-8C59D53A33C1}"/>
-    <hyperlink ref="C230" r:id="rId222" xr:uid="{691C9BD8-69D3-DA4B-AEB6-AF827B4ACA9F}"/>
-    <hyperlink ref="C231" r:id="rId223" xr:uid="{B6891E82-7C4D-424D-9219-3C9FD08E0053}"/>
-    <hyperlink ref="C232" r:id="rId224" xr:uid="{67A1AE98-62D2-644D-AC13-6CD76CF53CC0}"/>
-    <hyperlink ref="C233" r:id="rId225" xr:uid="{B59D4881-2A82-8F4D-B151-1E796C4923C8}"/>
-    <hyperlink ref="C234" r:id="rId226" xr:uid="{B3CBD023-5EFD-6048-9B3F-89F0C65CBBF5}"/>
-    <hyperlink ref="C235" r:id="rId227" xr:uid="{53EC42C4-22F7-0445-A0AC-7275A59A2672}"/>
-    <hyperlink ref="C236" r:id="rId228" xr:uid="{A29575F3-CB24-5B4B-9538-D5212B2DC28B}"/>
-    <hyperlink ref="C237" r:id="rId229" xr:uid="{353A44DD-9E30-8F48-8E2B-8DAA07550470}"/>
-    <hyperlink ref="C238" r:id="rId230" xr:uid="{32AC291D-95A5-BE49-88E0-02677BF39CAC}"/>
-    <hyperlink ref="C239" r:id="rId231" xr:uid="{A84F22FF-AD10-A546-8998-B066C0EB2D5A}"/>
-    <hyperlink ref="C240" r:id="rId232" xr:uid="{4C5CAF84-9B94-FC44-8C6C-B3CC7257C1DB}"/>
-    <hyperlink ref="C241" r:id="rId233" xr:uid="{5DA775E2-C516-3B47-8C82-3CEE7CC0BDF9}"/>
-    <hyperlink ref="C242" r:id="rId234" xr:uid="{00B6AE5C-EF3F-0747-A280-3BF055362B4F}"/>
-    <hyperlink ref="C243" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S." xr:uid="{BCBD0A7E-F3D0-E840-9375-AFD37C5CD41A}"/>
-    <hyperlink ref="C244" r:id="rId236" xr:uid="{47ABDDDB-F95F-8049-9FB3-1E71A7376DDE}"/>
-    <hyperlink ref="C245" r:id="rId237" xr:uid="{70BADFC9-7399-234D-99F6-4C5F02397C26}"/>
-    <hyperlink ref="C246" r:id="rId238" xr:uid="{63348580-70EF-EC47-BF49-8ECE9560D54E}"/>
-    <hyperlink ref="C247" r:id="rId239" xr:uid="{D5BD96B3-9EAB-1B47-AC87-5C47F6AD7F40}"/>
-    <hyperlink ref="C248" r:id="rId240" xr:uid="{74791141-3FB8-7540-B45B-9541AF0AE371}"/>
-    <hyperlink ref="C249" r:id="rId241" xr:uid="{88D53CD6-262A-7247-8E58-FE9FFF7ECC40}"/>
-    <hyperlink ref="C250" r:id="rId242" xr:uid="{4338A14D-4F7D-B943-A347-7F74EFCA0DB5}"/>
-    <hyperlink ref="C251" r:id="rId243" xr:uid="{6E0EF7A3-7341-284B-A0E3-4539B6EAFAF2}"/>
-    <hyperlink ref="C252" r:id="rId244" xr:uid="{D2D8D64F-E2D3-734E-AD45-3EFB9686555A}"/>
-    <hyperlink ref="C253" r:id="rId245" xr:uid="{04A2904A-73A0-7845-9868-2CCFE359AC68}"/>
-    <hyperlink ref="C254" r:id="rId246" xr:uid="{D3D35835-6BE3-4D41-AF6F-5FE442277A16}"/>
-    <hyperlink ref="C255" r:id="rId247" xr:uid="{F663D0FC-CFF0-BC4F-9D26-48C871A8E9FD}"/>
-    <hyperlink ref="C256" r:id="rId248" xr:uid="{DF544147-DA48-4041-A4E2-4A75106B771A}"/>
-    <hyperlink ref="C257" r:id="rId249" xr:uid="{50E4B716-239E-7946-843D-E8462591D128}"/>
-    <hyperlink ref="C258" r:id="rId250" xr:uid="{D368B3E5-7D12-FD48-AFF7-A4A614108940}"/>
-    <hyperlink ref="C259" r:id="rId251" xr:uid="{D5921FF1-FC1F-CA4B-A24E-AD69E1DEC14C}"/>
-    <hyperlink ref="C260" r:id="rId252" xr:uid="{C931D7E0-E032-7C4B-95F1-735D955FCB51}"/>
-    <hyperlink ref="C261" r:id="rId253" xr:uid="{5FBD4A8F-287C-2C46-9CAB-F7DBA67DEDDA}"/>
-    <hyperlink ref="C262" r:id="rId254" xr:uid="{12966DD6-41DD-A94B-8B2C-0AD7D2AD6FB0}"/>
-    <hyperlink ref="C263" r:id="rId255" xr:uid="{CF720C34-4554-2944-A818-020ABC9BF0F4}"/>
-    <hyperlink ref="C264" r:id="rId256" xr:uid="{75763F2A-16D7-DE43-8189-19623CE26370}"/>
-    <hyperlink ref="C265" r:id="rId257" xr:uid="{9263AA30-472A-0A4D-BADF-96D82BB9BFCC}"/>
-    <hyperlink ref="C266" r:id="rId258" xr:uid="{2EF025C3-75C8-564E-BA8B-708C32B0E602}"/>
-    <hyperlink ref="C267" r:id="rId259" xr:uid="{6BDFDCA9-3421-F24F-8EF2-A72742F0AC21}"/>
-    <hyperlink ref="C268" r:id="rId260" xr:uid="{D8447F99-5FF9-D544-99BB-E9969B4A38D7}"/>
-    <hyperlink ref="C269" r:id="rId261" xr:uid="{1DB7EFDA-6C7D-F546-9EE1-F61ED0F65209}"/>
-    <hyperlink ref="C270" r:id="rId262" xr:uid="{D1505609-27D1-784D-ACF6-AE9D0DA2E1B6}"/>
-    <hyperlink ref="C271" r:id="rId263" xr:uid="{6BFA7B45-17D0-4E49-85DA-23C7255A306D}"/>
-    <hyperlink ref="C272" r:id="rId264" xr:uid="{3324BA4A-30CA-5246-8C3C-6505A6987939}"/>
-    <hyperlink ref="C273" r:id="rId265" xr:uid="{894486AD-2B6D-5740-BCAF-0BA1AFF814B4}"/>
-    <hyperlink ref="C274" r:id="rId266" xr:uid="{C47B203B-8B5A-E740-8C86-0784AD28089E}"/>
-    <hyperlink ref="C275" r:id="rId267" xr:uid="{06DC2E54-7597-AE4D-ACDB-B8883A989A4F}"/>
-    <hyperlink ref="C276" r:id="rId268" xr:uid="{E3384259-7CA7-1C44-A66D-11346EE6742E}"/>
-    <hyperlink ref="C277" r:id="rId269" xr:uid="{A5B77769-38AF-3D47-A76B-311591B57D91}"/>
-    <hyperlink ref="C278" r:id="rId270" xr:uid="{9DB6976A-C646-1341-90E8-3A164521267A}"/>
-    <hyperlink ref="C279" r:id="rId271" xr:uid="{03C291F8-D19A-304B-9EF9-CF71A1F66E49}"/>
-    <hyperlink ref="C280" r:id="rId272" xr:uid="{7536415C-140B-9244-B0B2-23F3ED0B2D80}"/>
-    <hyperlink ref="C281" r:id="rId273" xr:uid="{7DBDA456-8AF6-DD43-9764-17D3959B8E8F}"/>
-    <hyperlink ref="C282" r:id="rId274" xr:uid="{BFC149AB-C15A-B648-9F6A-ECD3890B1918}"/>
-    <hyperlink ref="C283" r:id="rId275" xr:uid="{0482240B-FEE9-F746-8980-52BCB7BBB56E}"/>
-    <hyperlink ref="C284" r:id="rId276" xr:uid="{86D1231A-E7C8-4B45-99ED-2DB0EF71E190}"/>
-    <hyperlink ref="C285" r:id="rId277" xr:uid="{20B7CE89-CB37-0040-989F-C8D1BE2B8782}"/>
-    <hyperlink ref="C286" r:id="rId278" xr:uid="{4C8412C9-A47B-9244-A18B-741516BD1054}"/>
-    <hyperlink ref="C287" r:id="rId279" xr:uid="{511761D9-31CE-0B43-AFFD-C011C27ACC52}"/>
-    <hyperlink ref="C288" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)." xr:uid="{6905F997-D048-1049-BA27-C48756603D1E}"/>
-    <hyperlink ref="C289" r:id="rId281" xr:uid="{E657AA82-7CFE-DB42-B20F-F63D8C25EAB6}"/>
-    <hyperlink ref="C290" r:id="rId282" xr:uid="{3E505033-58F3-8F4E-AB82-E12DBC226AEA}"/>
-    <hyperlink ref="C291" r:id="rId283" xr:uid="{749599E5-4972-7343-B13B-87E26F837470}"/>
-    <hyperlink ref="C292" r:id="rId284" xr:uid="{12AA88DC-22AB-5A49-B28C-F04C8E35A215}"/>
-    <hyperlink ref="C293" r:id="rId285" xr:uid="{5751F0A7-7D9D-4148-820B-5B9659DFE34F}"/>
-    <hyperlink ref="C294" r:id="rId286" xr:uid="{4CA2DBEE-B161-B84D-B3A9-B8BC1B598AF2}"/>
-    <hyperlink ref="C295" r:id="rId287" xr:uid="{A9C1E578-6594-954C-8785-8902E605FC7A}"/>
-    <hyperlink ref="C296" r:id="rId288" xr:uid="{3D45E9B8-6671-A747-8C18-51CF8883170A}"/>
-    <hyperlink ref="C297" r:id="rId289" xr:uid="{4F5EF748-8CD4-0F47-90CE-3C93755BF63D}"/>
-    <hyperlink ref="C298" r:id="rId290" xr:uid="{44053C08-5050-C84B-B016-069B1EF9A43D}"/>
-    <hyperlink ref="C299" r:id="rId291" xr:uid="{ABF38928-736B-1A49-8B8A-1DCA5AAECB2B}"/>
-    <hyperlink ref="C300" r:id="rId292" xr:uid="{52651FAF-F3DC-E949-8AF8-998B9724B7D1}"/>
-    <hyperlink ref="C301" r:id="rId293" xr:uid="{91C6CCEF-3FF7-2C42-B5A0-8F4A403ED198}"/>
-    <hyperlink ref="C302" r:id="rId294" xr:uid="{15C8AF08-1A79-F949-9BE7-DD240CBD9861}"/>
-    <hyperlink ref="C303" r:id="rId295" xr:uid="{1904F984-5B22-8D46-BC33-3073B390E8F9}"/>
-    <hyperlink ref="C304" r:id="rId296" xr:uid="{A8BFB3A4-426B-E646-BCF0-FE19C8CD07A9}"/>
-    <hyperlink ref="C305" r:id="rId297" xr:uid="{FBBA29BB-885B-744A-A644-58EDCA7B140A}"/>
-    <hyperlink ref="C306" r:id="rId298" xr:uid="{75411687-6884-AC42-8B4A-1348C4837365}"/>
-    <hyperlink ref="C307" r:id="rId299" xr:uid="{A89ED8DF-F678-FE43-808C-C190721379BF}"/>
-    <hyperlink ref="C308" r:id="rId300" xr:uid="{1516834D-F3B2-1743-8811-263E11BBDEF8}"/>
-    <hyperlink ref="C309" r:id="rId301" xr:uid="{1659AB91-08CA-E44D-988D-E9D9A746D406}"/>
-    <hyperlink ref="C310" r:id="rId302" xr:uid="{E844BC1D-9713-9F4D-B0A4-1124A9952D14}"/>
-    <hyperlink ref="C311" r:id="rId303" xr:uid="{DCE2AAEF-8D8E-1843-BFE9-E9B7E13854EB}"/>
-    <hyperlink ref="C312" r:id="rId304" xr:uid="{836B3BF0-7711-7D41-9E72-914C1871397F}"/>
-    <hyperlink ref="C313" r:id="rId305" xr:uid="{F450CF9B-CA59-1443-8163-13F1121DCF12}"/>
-    <hyperlink ref="C314" r:id="rId306" xr:uid="{1539C3E8-4854-3C4F-A7B3-55BF931F1E2A}"/>
-    <hyperlink ref="C315" r:id="rId307" xr:uid="{04F1FC5F-5DA1-0144-962D-B38C1C41F0F4}"/>
-    <hyperlink ref="C316" r:id="rId308" xr:uid="{B21618F4-70E2-C549-80B7-7CF915679E0A}"/>
-    <hyperlink ref="C317" r:id="rId309" xr:uid="{EEDFBF11-C1E4-0847-9D56-94A72D97AEE7}"/>
-    <hyperlink ref="C318" r:id="rId310" xr:uid="{F5C0EDF1-7EAC-8849-8D27-C3389913BFC6}"/>
-    <hyperlink ref="C319" r:id="rId311" xr:uid="{50175B29-124F-4E4E-8E98-961BD3320359}"/>
-    <hyperlink ref="C320" r:id="rId312" xr:uid="{1BE23822-8512-014F-9154-F6EDA4FC8428}"/>
-    <hyperlink ref="C321" r:id="rId313" xr:uid="{38EC228E-ABFF-3542-9CFB-3DDFC628E9D0}"/>
-    <hyperlink ref="C322" r:id="rId314" xr:uid="{73F240F8-C469-454E-BA5C-CFF2F7A7A5F6}"/>
-    <hyperlink ref="C323" r:id="rId315" xr:uid="{3BBD1BAC-68C7-A94A-9063-AF62B5C837FD}"/>
-    <hyperlink ref="C324" r:id="rId316" xr:uid="{F9751D9B-2689-E24B-9FC3-CA32FE888708}"/>
-    <hyperlink ref="C325" r:id="rId317" xr:uid="{73C61D6A-D97C-B944-8B27-BB91564AB0D7}"/>
-    <hyperlink ref="C326" r:id="rId318" xr:uid="{936E077C-C016-A04F-895A-782D6D9D9433}"/>
-    <hyperlink ref="C327" r:id="rId319" xr:uid="{5454A2A1-6607-BE48-9215-CB8965EC3568}"/>
-    <hyperlink ref="C328" r:id="rId320" xr:uid="{FC1EAA10-F7ED-6B42-A79B-3D8B44E2C8B3}"/>
-    <hyperlink ref="C329" r:id="rId321" xr:uid="{FDB7F712-4A42-1048-8929-A1E752B07C6A}"/>
-    <hyperlink ref="C330" r:id="rId322" xr:uid="{AF3ACA60-0B0E-E146-B51F-A2CD05EB6549}"/>
-    <hyperlink ref="C331" r:id="rId323" xr:uid="{BB63E040-7A1A-E046-9BDD-9CBD1DA89DE9}"/>
-    <hyperlink ref="C332" r:id="rId324" xr:uid="{9AF8FD93-CCC9-D540-AE9A-00583F309649}"/>
-    <hyperlink ref="C333" r:id="rId325" xr:uid="{66A746A0-71FE-E546-92B7-D1C3D582E067}"/>
-    <hyperlink ref="C335" r:id="rId326" xr:uid="{BD79CCE1-5315-3944-9F9B-618615EC4583}"/>
-    <hyperlink ref="C336" r:id="rId327" xr:uid="{A5068A51-C961-6847-BB27-40A850B6D393}"/>
-    <hyperlink ref="C337" r:id="rId328" xr:uid="{6B8D36F0-E796-B944-A456-E8A9E2EE0BDB}"/>
-    <hyperlink ref="C338" r:id="rId329" xr:uid="{776652B7-2C11-4641-BF6A-EABEEB9B55AB}"/>
-    <hyperlink ref="C339" r:id="rId330" xr:uid="{95C6B35D-712A-2343-B790-236B55C5EC49}"/>
-    <hyperlink ref="C340" r:id="rId331" xr:uid="{4ED53872-1FE9-F140-AA35-F228F762880B}"/>
-    <hyperlink ref="C341" r:id="rId332" xr:uid="{6D5E6A28-85AA-BF4C-B2BD-9378D6E28EC7}"/>
-    <hyperlink ref="C342" r:id="rId333" xr:uid="{BCAD1ECB-15EE-CF49-878E-AA682DE3AC22}"/>
-    <hyperlink ref="C343" r:id="rId334" xr:uid="{C85468B5-25E9-E446-808E-72CFE911F0C2}"/>
-    <hyperlink ref="C344" r:id="rId335" xr:uid="{9503AECA-1A6A-9640-A04C-4CEAA2304448}"/>
-    <hyperlink ref="C345" r:id="rId336" xr:uid="{74211516-06B0-AA45-845B-52C8202751DA}"/>
-    <hyperlink ref="C346" r:id="rId337" xr:uid="{02C696BC-4B91-9444-900F-9CD68E409ABC}"/>
-    <hyperlink ref="C347" r:id="rId338" xr:uid="{04646C45-4118-374C-839D-94D31D534FAC}"/>
-    <hyperlink ref="C348" r:id="rId339" xr:uid="{F90BCCAE-8596-FC4D-BDD7-774392C596DF}"/>
-    <hyperlink ref="C349" r:id="rId340" xr:uid="{65230925-36EC-8A4B-8E46-6350B9BC0F95}"/>
-    <hyperlink ref="C350" r:id="rId341" xr:uid="{E91B8177-0C7A-1F40-BD34-4CC60F03B84F}"/>
-    <hyperlink ref="C351" r:id="rId342" xr:uid="{E8CBFD60-7335-0B4D-9FF5-99B4A8DC551D}"/>
-    <hyperlink ref="C352" r:id="rId343" xr:uid="{A35F55D4-9B87-C745-94DB-E7D820193C30}"/>
-    <hyperlink ref="C353" r:id="rId344" xr:uid="{6461A29F-D404-334F-B13F-296B4CA5E8A4}"/>
-    <hyperlink ref="C354" r:id="rId345" xr:uid="{FA9B4BE7-85CC-B24F-9461-5E9B42DDD824}"/>
-    <hyperlink ref="C355" r:id="rId346" xr:uid="{A75ACEA2-CDF6-A147-8540-A6DF55B15F45}"/>
-    <hyperlink ref="C356" r:id="rId347" xr:uid="{62FF87E2-E658-AB4D-AC57-7BCF9D49516E}"/>
-    <hyperlink ref="C357" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color." xr:uid="{269338A6-5145-6944-9F7F-BD2A86DFA308}"/>
-    <hyperlink ref="C358" r:id="rId349" xr:uid="{8F583049-CE8D-CD42-88CD-CF3857942670}"/>
-    <hyperlink ref="C359" r:id="rId350" xr:uid="{EE2348AD-E296-894A-B5AE-5884A3C5E419}"/>
-    <hyperlink ref="C360" r:id="rId351" xr:uid="{6EACB34E-B32E-8F43-8055-2406F7417A7E}"/>
-    <hyperlink ref="C361" r:id="rId352" xr:uid="{2446F10A-B762-B64C-97B2-6131A0BECC1F}"/>
-    <hyperlink ref="C362" r:id="rId353" xr:uid="{6FDFCC53-17A6-7244-88A7-49406D7C9200}"/>
-    <hyperlink ref="C363" r:id="rId354" xr:uid="{3EC43646-EAB1-E443-A2F6-8E6E5FC77083}"/>
-    <hyperlink ref="C364" r:id="rId355" xr:uid="{659D9F20-C862-C947-B422-84143CFE317F}"/>
-    <hyperlink ref="C365" r:id="rId356" xr:uid="{3F5192FE-1C50-C049-88D5-68FA0F5430A0}"/>
-    <hyperlink ref="C366" r:id="rId357" xr:uid="{5EAD7CDA-9545-454B-BE77-9AFEC6AC1083}"/>
-    <hyperlink ref="C367" r:id="rId358" xr:uid="{761E5451-736B-6745-9CF5-4C6EF5D4C099}"/>
-    <hyperlink ref="C368" r:id="rId359" xr:uid="{4C8677A9-D94C-134F-AF31-E424751BF867}"/>
-    <hyperlink ref="C369" r:id="rId360" xr:uid="{CCF7920F-D5CE-004A-86C3-D821FB230970}"/>
-    <hyperlink ref="C370" r:id="rId361" xr:uid="{B4C07A0A-1EDD-7947-9646-3FD603441AD7}"/>
-    <hyperlink ref="C371" r:id="rId362" xr:uid="{49F7BB43-6851-0641-9DC5-27DBC66706F6}"/>
-    <hyperlink ref="C372" r:id="rId363" xr:uid="{77038647-48C7-5547-8E0F-898610362465}"/>
-    <hyperlink ref="C374" r:id="rId364" xr:uid="{EEFFE19C-6571-C64F-A0E1-5A4A700D94D4}"/>
-    <hyperlink ref="C373" r:id="rId365" xr:uid="{A4A2BFC4-6B88-2E4E-B362-17D8EE041C89}"/>
-    <hyperlink ref="C375" r:id="rId366" xr:uid="{DC5B603A-8D65-3648-A08A-E5FFA0FAE879}"/>
-    <hyperlink ref="C376" r:id="rId367" xr:uid="{F8807DD9-F4F2-B147-9C31-DBC93B2E477B}"/>
-    <hyperlink ref="C377" r:id="rId368" xr:uid="{6F7B396C-D7E9-C04E-BAE2-53D2EE07172B}"/>
-    <hyperlink ref="C378" r:id="rId369" xr:uid="{0D4A5941-C669-4A49-BAE3-9B553D03BD0F}"/>
-    <hyperlink ref="C379" r:id="rId370" xr:uid="{54144336-5BCA-D749-962A-E448C2CED3D3}"/>
-    <hyperlink ref="C380" r:id="rId371" xr:uid="{3A41DD21-CACF-1F48-A7C7-F568C6F31F3E}"/>
-    <hyperlink ref="C381" r:id="rId372" xr:uid="{A36160A8-F45E-3443-9645-42C1004B8F8C}"/>
-    <hyperlink ref="C382" r:id="rId373" xr:uid="{8B0A00A3-6AC0-DF46-AD87-A4DA016A2A00}"/>
-    <hyperlink ref="C383" r:id="rId374" xr:uid="{62A81CB4-A961-C543-B31C-92059DB6C105}"/>
-    <hyperlink ref="C384" r:id="rId375" xr:uid="{08030975-009C-C34A-A875-72FE2718F44C}"/>
-    <hyperlink ref="C385" r:id="rId376" xr:uid="{A113C7A9-2359-B643-9C08-E845813439C0}"/>
-    <hyperlink ref="C386" r:id="rId377" xr:uid="{FE300343-4633-AD47-A64D-2086629EB398}"/>
-    <hyperlink ref="C387" r:id="rId378" xr:uid="{4FC9F782-D38F-C642-A863-887B17AD05CD}"/>
-    <hyperlink ref="C388" r:id="rId379" xr:uid="{830C5466-10E3-7A48-B3E7-35C15A1CA4EF}"/>
-    <hyperlink ref="C389" r:id="rId380" xr:uid="{1B987077-E9D3-6F40-89EE-0D4E7180D884}"/>
-    <hyperlink ref="C390" r:id="rId381" xr:uid="{D4843E1F-7226-864E-A4BB-264D5A487B6D}"/>
-    <hyperlink ref="C391" r:id="rId382" xr:uid="{61816592-2D19-9946-8253-47A60218F2EA}"/>
-    <hyperlink ref="C392" r:id="rId383" xr:uid="{736C840F-19A3-0A4B-8863-ECB772B46385}"/>
-    <hyperlink ref="C393" r:id="rId384" xr:uid="{05A238AD-3C5B-C546-94E9-75BBF964711A}"/>
-    <hyperlink ref="C394" r:id="rId385" xr:uid="{7029629C-3F2A-4A49-997B-CFE86EC8B3C2}"/>
-    <hyperlink ref="C395" r:id="rId386" xr:uid="{ADA66B57-2FAC-AB42-BD83-4931708F3AB5}"/>
-    <hyperlink ref="C396" r:id="rId387" xr:uid="{F16BF1F9-755B-B045-B9A8-0B97E3BAC8B0}"/>
-    <hyperlink ref="C397" r:id="rId388" xr:uid="{ECCE930A-B960-234C-81EC-4B8514282AE9}"/>
-    <hyperlink ref="C398" r:id="rId389" xr:uid="{7AA58141-7D24-7C42-A0C1-F852B21CFFD9}"/>
-    <hyperlink ref="C399" r:id="rId390" xr:uid="{B1FCB47D-7921-3446-B2C7-72CBA815D056}"/>
-    <hyperlink ref="C400" r:id="rId391" xr:uid="{8C547719-AA03-3543-B31F-7300674AF4C5}"/>
-    <hyperlink ref="C401" r:id="rId392" xr:uid="{09922668-AFC0-F242-860E-9967E0F0FEF4}"/>
-    <hyperlink ref="C402" r:id="rId393" xr:uid="{0DA963DA-238B-D44E-9E03-6E6BD933B35E}"/>
-    <hyperlink ref="C403" r:id="rId394" xr:uid="{89518AFF-2526-C845-BC9D-95FE77AF416E}"/>
-    <hyperlink ref="C404" r:id="rId395" xr:uid="{FAECBBBE-196C-7A41-A0FB-E0597CB2CF51}"/>
-    <hyperlink ref="C405" r:id="rId396" xr:uid="{8126B039-0B25-B040-A0F6-C3457341A2E9}"/>
-    <hyperlink ref="C406" r:id="rId397" xr:uid="{6CB326E6-E698-EB42-884B-C89FFA33E3BA}"/>
-    <hyperlink ref="C407" r:id="rId398" xr:uid="{8C97EFD1-933F-A44F-A1CF-6386233104A2}"/>
-    <hyperlink ref="C408" r:id="rId399" xr:uid="{8F019F07-8532-E147-8BE1-4EBE833F61CA}"/>
-    <hyperlink ref="C409" r:id="rId400" xr:uid="{00F1A08F-3767-784A-97A3-4603DE38BACC}"/>
-    <hyperlink ref="C410" r:id="rId401" xr:uid="{2A84ADCB-071F-9A48-994D-7A838307EFD8}"/>
-    <hyperlink ref="C411" r:id="rId402" xr:uid="{132F8C6D-D5E8-6440-AC4E-B81EA2100416}"/>
-    <hyperlink ref="C412" r:id="rId403" xr:uid="{2DA6EAC2-1A1D-754F-9613-226CBC7890AF}"/>
-    <hyperlink ref="C413" r:id="rId404" xr:uid="{05BED99A-4562-D14E-8627-D07CF5335A9B}"/>
-    <hyperlink ref="C414" r:id="rId405" xr:uid="{111D902A-3F60-2D4B-89D3-5BCBD8AA38DD}"/>
-    <hyperlink ref="C415" r:id="rId406" xr:uid="{F19236BE-AC32-3542-9214-DFC3BAE04ED0}"/>
-    <hyperlink ref="C416" r:id="rId407" xr:uid="{4D97CD96-EA1B-664E-9380-EFD27077D273}"/>
-    <hyperlink ref="C417" r:id="rId408" xr:uid="{49A46D91-633F-A148-ACFA-49B7D1AA4B33}"/>
-    <hyperlink ref="C418" r:id="rId409" xr:uid="{7C3B7901-67E3-EA4D-BC64-21A78BC03AC6}"/>
-    <hyperlink ref="C419" r:id="rId410" xr:uid="{B27CA8C3-D34F-5E4D-94A5-11D14AFD0F82}"/>
-    <hyperlink ref="C420" r:id="rId411" xr:uid="{8FECE038-9764-5E4A-8C6E-9B3209812651}"/>
-    <hyperlink ref="C421" r:id="rId412" xr:uid="{95696D4B-89CB-5640-BE92-53B3C043F7EB}"/>
-    <hyperlink ref="C422" r:id="rId413" xr:uid="{DA74B737-802A-4944-A93E-0B9C8417630B}"/>
-    <hyperlink ref="C423" r:id="rId414" xr:uid="{B2C4C168-50FA-AF41-8F56-9E70613CF17D}"/>
-    <hyperlink ref="C425" r:id="rId415" xr:uid="{B7090C60-AC27-3F4F-8F0D-42F0791928C6}"/>
-    <hyperlink ref="C424" r:id="rId416" xr:uid="{07400041-66C6-514B-B3E3-427F2947C2B7}"/>
-    <hyperlink ref="C426" r:id="rId417" xr:uid="{B7E78172-8FB8-4E42-87D8-6A4654D79C62}"/>
-    <hyperlink ref="C427" r:id="rId418" xr:uid="{9A5D4670-BC64-334A-88CF-6F8287692C5E}"/>
-    <hyperlink ref="C428" r:id="rId419" xr:uid="{604283B6-53BC-044F-8D9D-E6094E798317}"/>
-    <hyperlink ref="C429" r:id="rId420" xr:uid="{5EB15AC7-3E0E-E44C-A5B9-32F30F234B5A}"/>
-    <hyperlink ref="C430" r:id="rId421" xr:uid="{3076BD5F-4B23-4146-A50A-499C9FF4C3D2}"/>
-    <hyperlink ref="C431" r:id="rId422" xr:uid="{6A29D9C2-1E78-1B43-A251-0AB0A97FA70E}"/>
-    <hyperlink ref="C432" r:id="rId423" xr:uid="{00597D5E-D693-DF4E-84C0-47E58A6ACA8F}"/>
-    <hyperlink ref="C433" r:id="rId424" xr:uid="{48640988-9964-0B4C-A014-83E2CEB3D632}"/>
-    <hyperlink ref="C434" r:id="rId425" xr:uid="{617AADC9-7534-FE45-96B0-EF4C1867B793}"/>
-    <hyperlink ref="C435" r:id="rId426" xr:uid="{7F8CDAA4-5094-8E4E-961B-41CDE5ACC0C0}"/>
-    <hyperlink ref="C436" r:id="rId427" xr:uid="{63F28ABD-12CF-5947-80DA-229E3CA3133E}"/>
-    <hyperlink ref="C443" r:id="rId428" xr:uid="{0A1DB92C-3315-1942-B27D-4B90986A6D9D}"/>
-    <hyperlink ref="C442" r:id="rId429" xr:uid="{11738B67-CADD-5D45-8417-8BE7A03FC79F}"/>
-    <hyperlink ref="C441" r:id="rId430" xr:uid="{B2B23748-D9E4-BE4F-A93E-49ECB4063831}"/>
-    <hyperlink ref="C440" r:id="rId431" xr:uid="{A2FB8A72-37B9-7E4A-B050-FD6CD20BCE73}"/>
-    <hyperlink ref="C439" r:id="rId432" xr:uid="{5A93C9AF-BFEB-EB40-95AC-C309ED09A604}"/>
-    <hyperlink ref="C438" r:id="rId433" xr:uid="{CC203923-2DC2-874B-B846-A8455E3CC2F2}"/>
-    <hyperlink ref="C437" r:id="rId434" xr:uid="{FCB0246E-0179-B447-B3CE-C60CDB388472}"/>
-    <hyperlink ref="C444" r:id="rId435" xr:uid="{F06CEE72-8CA4-C547-862C-39B86CD3226A}"/>
-    <hyperlink ref="C445" r:id="rId436" xr:uid="{CB3045F2-8D63-0F4E-85BC-AF016DB4F247}"/>
-    <hyperlink ref="C446" r:id="rId437" xr:uid="{667D57F5-E5AD-674F-A2F5-AFF4A14E4026}"/>
-    <hyperlink ref="C447" r:id="rId438" xr:uid="{27A13A65-56CE-BF4D-BA0D-EB87D910272D}"/>
-    <hyperlink ref="C448" r:id="rId439" xr:uid="{2C72A52E-6F06-0246-AEB5-93CD0DEA8866}"/>
-    <hyperlink ref="C449" r:id="rId440" xr:uid="{24B29046-B4DD-674B-9EDF-6C94BEC3FDD8}"/>
-    <hyperlink ref="C450" r:id="rId441" xr:uid="{D018EBC3-3FB3-AC4D-9D64-D218345A46C8}"/>
-    <hyperlink ref="C453" r:id="rId442" xr:uid="{1E1D3964-01E0-3145-ACFE-B6A5BF0EECB0}"/>
-    <hyperlink ref="C451" r:id="rId443" xr:uid="{FA0E5061-A7E2-C045-9671-1CD9446D1932}"/>
-    <hyperlink ref="C452" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result." xr:uid="{92704F5B-7B31-2F42-80DD-764B2206D9DB}"/>
-    <hyperlink ref="C334" r:id="rId445" xr:uid="{A48B1A24-83B1-7A4C-8129-CD37804DF849}"/>
-    <hyperlink ref="C2" r:id="rId446" xr:uid="{E07D4FE5-46C7-AC4D-9E01-2300AA43B58A}"/>
+    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C9" r:id="rId4"/>
+    <hyperlink ref="C10" r:id="rId5"/>
+    <hyperlink ref="C11" r:id="rId6"/>
+    <hyperlink ref="C12" r:id="rId7"/>
+    <hyperlink ref="C13" r:id="rId8"/>
+    <hyperlink ref="C14" r:id="rId9"/>
+    <hyperlink ref="C15" r:id="rId10"/>
+    <hyperlink ref="C16" r:id="rId11"/>
+    <hyperlink ref="C17" r:id="rId12"/>
+    <hyperlink ref="C18" r:id="rId13"/>
+    <hyperlink ref="C19" r:id="rId14"/>
+    <hyperlink ref="C20" r:id="rId15"/>
+    <hyperlink ref="C21" r:id="rId16"/>
+    <hyperlink ref="C22" r:id="rId17"/>
+    <hyperlink ref="C23" r:id="rId18"/>
+    <hyperlink ref="C24" r:id="rId19"/>
+    <hyperlink ref="C25" r:id="rId20"/>
+    <hyperlink ref="C26" r:id="rId21"/>
+    <hyperlink ref="C27" r:id="rId22"/>
+    <hyperlink ref="C28" r:id="rId23"/>
+    <hyperlink ref="C29" r:id="rId24"/>
+    <hyperlink ref="C30" r:id="rId25"/>
+    <hyperlink ref="C31" r:id="rId26"/>
+    <hyperlink ref="C32" r:id="rId27"/>
+    <hyperlink ref="C33" r:id="rId28"/>
+    <hyperlink ref="C34" r:id="rId29"/>
+    <hyperlink ref="C35" r:id="rId30"/>
+    <hyperlink ref="C36" r:id="rId31"/>
+    <hyperlink ref="C37" r:id="rId32"/>
+    <hyperlink ref="C38" r:id="rId33"/>
+    <hyperlink ref="C39" r:id="rId34"/>
+    <hyperlink ref="C40" r:id="rId35"/>
+    <hyperlink ref="C41" r:id="rId36"/>
+    <hyperlink ref="C42" r:id="rId37"/>
+    <hyperlink ref="C43" r:id="rId38"/>
+    <hyperlink ref="C44" r:id="rId39"/>
+    <hyperlink ref="C45" r:id="rId40"/>
+    <hyperlink ref="C46" r:id="rId41"/>
+    <hyperlink ref="C47" r:id="rId42"/>
+    <hyperlink ref="C48" r:id="rId43"/>
+    <hyperlink ref="C49" r:id="rId44"/>
+    <hyperlink ref="C50" r:id="rId45"/>
+    <hyperlink ref="C51" r:id="rId46"/>
+    <hyperlink ref="C52" r:id="rId47"/>
+    <hyperlink ref="C53" r:id="rId48"/>
+    <hyperlink ref="C54" r:id="rId49"/>
+    <hyperlink ref="C56" r:id="rId50"/>
+    <hyperlink ref="C57" r:id="rId51"/>
+    <hyperlink ref="C58" r:id="rId52"/>
+    <hyperlink ref="C59" r:id="rId53"/>
+    <hyperlink ref="C60" r:id="rId54"/>
+    <hyperlink ref="C61" r:id="rId55"/>
+    <hyperlink ref="C62" r:id="rId56"/>
+    <hyperlink ref="C63" r:id="rId57"/>
+    <hyperlink ref="C64" r:id="rId58"/>
+    <hyperlink ref="C65" r:id="rId59"/>
+    <hyperlink ref="C66" r:id="rId60"/>
+    <hyperlink ref="C67" r:id="rId61"/>
+    <hyperlink ref="C68" r:id="rId62"/>
+    <hyperlink ref="C69" r:id="rId63"/>
+    <hyperlink ref="C70" r:id="rId64"/>
+    <hyperlink ref="C71" r:id="rId65"/>
+    <hyperlink ref="C72" r:id="rId66"/>
+    <hyperlink ref="C73" r:id="rId67"/>
+    <hyperlink ref="C74" r:id="rId68"/>
+    <hyperlink ref="C75" r:id="rId69"/>
+    <hyperlink ref="C76" r:id="rId70"/>
+    <hyperlink ref="C77" r:id="rId71"/>
+    <hyperlink ref="C78" r:id="rId72"/>
+    <hyperlink ref="C79" r:id="rId73"/>
+    <hyperlink ref="C80" r:id="rId74"/>
+    <hyperlink ref="C81" r:id="rId75"/>
+    <hyperlink ref="C82" r:id="rId76"/>
+    <hyperlink ref="C83" r:id="rId77"/>
+    <hyperlink ref="C84" r:id="rId78"/>
+    <hyperlink ref="C85" r:id="rId79"/>
+    <hyperlink ref="C86" r:id="rId80"/>
+    <hyperlink ref="C87" r:id="rId81"/>
+    <hyperlink ref="C88" r:id="rId82"/>
+    <hyperlink ref="C89" r:id="rId83"/>
+    <hyperlink ref="C90" r:id="rId84"/>
+    <hyperlink ref="C91" r:id="rId85"/>
+    <hyperlink ref="C92" r:id="rId86"/>
+    <hyperlink ref="C93" r:id="rId87"/>
+    <hyperlink ref="C94" r:id="rId88"/>
+    <hyperlink ref="C95" r:id="rId89"/>
+    <hyperlink ref="C96" r:id="rId90"/>
+    <hyperlink ref="C97" r:id="rId91"/>
+    <hyperlink ref="C98" r:id="rId92"/>
+    <hyperlink ref="C100" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
+    <hyperlink ref="C101" r:id="rId94"/>
+    <hyperlink ref="C102" r:id="rId95"/>
+    <hyperlink ref="C103" r:id="rId96"/>
+    <hyperlink ref="C104" r:id="rId97"/>
+    <hyperlink ref="C105" r:id="rId98"/>
+    <hyperlink ref="C107" r:id="rId99"/>
+    <hyperlink ref="C108" r:id="rId100"/>
+    <hyperlink ref="C109" r:id="rId101"/>
+    <hyperlink ref="C110" r:id="rId102"/>
+    <hyperlink ref="C111" r:id="rId103"/>
+    <hyperlink ref="C112" r:id="rId104"/>
+    <hyperlink ref="C113" r:id="rId105"/>
+    <hyperlink ref="C114" r:id="rId106"/>
+    <hyperlink ref="C115" r:id="rId107"/>
+    <hyperlink ref="C116" r:id="rId108"/>
+    <hyperlink ref="C117" r:id="rId109"/>
+    <hyperlink ref="C118" r:id="rId110"/>
+    <hyperlink ref="C119" r:id="rId111"/>
+    <hyperlink ref="C120" r:id="rId112"/>
+    <hyperlink ref="C121" r:id="rId113"/>
+    <hyperlink ref="C122" r:id="rId114"/>
+    <hyperlink ref="C123" r:id="rId115"/>
+    <hyperlink ref="C124" r:id="rId116"/>
+    <hyperlink ref="C125" r:id="rId117"/>
+    <hyperlink ref="C126" r:id="rId118"/>
+    <hyperlink ref="C127" r:id="rId119"/>
+    <hyperlink ref="C128" r:id="rId120"/>
+    <hyperlink ref="C129" r:id="rId121"/>
+    <hyperlink ref="C130" r:id="rId122"/>
+    <hyperlink ref="C99" r:id="rId123"/>
+    <hyperlink ref="C106" r:id="rId124"/>
+    <hyperlink ref="C131" r:id="rId125"/>
+    <hyperlink ref="C132" r:id="rId126"/>
+    <hyperlink ref="C133" r:id="rId127"/>
+    <hyperlink ref="C134" r:id="rId128"/>
+    <hyperlink ref="C135" r:id="rId129"/>
+    <hyperlink ref="C136" r:id="rId130"/>
+    <hyperlink ref="C137" r:id="rId131"/>
+    <hyperlink ref="C138" r:id="rId132"/>
+    <hyperlink ref="C139" r:id="rId133"/>
+    <hyperlink ref="C140" r:id="rId134"/>
+    <hyperlink ref="C141" r:id="rId135"/>
+    <hyperlink ref="C142" r:id="rId136"/>
+    <hyperlink ref="C143" r:id="rId137"/>
+    <hyperlink ref="C144" r:id="rId138"/>
+    <hyperlink ref="C145" r:id="rId139"/>
+    <hyperlink ref="C146" r:id="rId140"/>
+    <hyperlink ref="C147" r:id="rId141"/>
+    <hyperlink ref="C148" r:id="rId142"/>
+    <hyperlink ref="C149" r:id="rId143"/>
+    <hyperlink ref="C150" r:id="rId144"/>
+    <hyperlink ref="C151" r:id="rId145"/>
+    <hyperlink ref="C152" r:id="rId146"/>
+    <hyperlink ref="C153" r:id="rId147"/>
+    <hyperlink ref="C154" r:id="rId148"/>
+    <hyperlink ref="C155" r:id="rId149"/>
+    <hyperlink ref="C158" r:id="rId150"/>
+    <hyperlink ref="C159" r:id="rId151"/>
+    <hyperlink ref="C160" r:id="rId152"/>
+    <hyperlink ref="C161" r:id="rId153"/>
+    <hyperlink ref="C162" r:id="rId154"/>
+    <hyperlink ref="C163" r:id="rId155"/>
+    <hyperlink ref="C164" r:id="rId156"/>
+    <hyperlink ref="C165" r:id="rId157"/>
+    <hyperlink ref="C166" r:id="rId158"/>
+    <hyperlink ref="C167" r:id="rId159"/>
+    <hyperlink ref="C168" r:id="rId160"/>
+    <hyperlink ref="C169" r:id="rId161"/>
+    <hyperlink ref="C170" r:id="rId162"/>
+    <hyperlink ref="C171" r:id="rId163"/>
+    <hyperlink ref="C172" r:id="rId164"/>
+    <hyperlink ref="C173" r:id="rId165"/>
+    <hyperlink ref="C174" r:id="rId166"/>
+    <hyperlink ref="C175" r:id="rId167"/>
+    <hyperlink ref="C176" r:id="rId168"/>
+    <hyperlink ref="C177" r:id="rId169"/>
+    <hyperlink ref="C178" r:id="rId170"/>
+    <hyperlink ref="C179" r:id="rId171"/>
+    <hyperlink ref="C180" r:id="rId172"/>
+    <hyperlink ref="C181" r:id="rId173"/>
+    <hyperlink ref="C182" r:id="rId174"/>
+    <hyperlink ref="C183" r:id="rId175"/>
+    <hyperlink ref="C184" r:id="rId176"/>
+    <hyperlink ref="C185" r:id="rId177"/>
+    <hyperlink ref="C186" r:id="rId178"/>
+    <hyperlink ref="C187" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="C188" r:id="rId180"/>
+    <hyperlink ref="C189" r:id="rId181"/>
+    <hyperlink ref="C190" r:id="rId182"/>
+    <hyperlink ref="C191" r:id="rId183"/>
+    <hyperlink ref="C192" r:id="rId184"/>
+    <hyperlink ref="C193" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="C194" r:id="rId186"/>
+    <hyperlink ref="C195" r:id="rId187"/>
+    <hyperlink ref="C196" r:id="rId188"/>
+    <hyperlink ref="C197" r:id="rId189"/>
+    <hyperlink ref="C198" r:id="rId190"/>
+    <hyperlink ref="C199" r:id="rId191"/>
+    <hyperlink ref="C200" r:id="rId192"/>
+    <hyperlink ref="C201" r:id="rId193"/>
+    <hyperlink ref="C202" r:id="rId194"/>
+    <hyperlink ref="C203" r:id="rId195"/>
+    <hyperlink ref="C204" r:id="rId196"/>
+    <hyperlink ref="C205" r:id="rId197"/>
+    <hyperlink ref="C206" r:id="rId198"/>
+    <hyperlink ref="C207" r:id="rId199"/>
+    <hyperlink ref="C208" r:id="rId200"/>
+    <hyperlink ref="C209" r:id="rId201"/>
+    <hyperlink ref="C210" r:id="rId202"/>
+    <hyperlink ref="C211" r:id="rId203"/>
+    <hyperlink ref="C212" r:id="rId204"/>
+    <hyperlink ref="C213" r:id="rId205"/>
+    <hyperlink ref="C214" r:id="rId206"/>
+    <hyperlink ref="C215" r:id="rId207"/>
+    <hyperlink ref="C216" r:id="rId208"/>
+    <hyperlink ref="C217" r:id="rId209"/>
+    <hyperlink ref="C218" r:id="rId210"/>
+    <hyperlink ref="C219" r:id="rId211"/>
+    <hyperlink ref="C220" r:id="rId212"/>
+    <hyperlink ref="C221" r:id="rId213"/>
+    <hyperlink ref="C222" r:id="rId214"/>
+    <hyperlink ref="C223" r:id="rId215"/>
+    <hyperlink ref="C224" r:id="rId216"/>
+    <hyperlink ref="C225" r:id="rId217"/>
+    <hyperlink ref="C226" r:id="rId218"/>
+    <hyperlink ref="C227" r:id="rId219"/>
+    <hyperlink ref="C228" r:id="rId220"/>
+    <hyperlink ref="C229" r:id="rId221"/>
+    <hyperlink ref="C230" r:id="rId222"/>
+    <hyperlink ref="C231" r:id="rId223"/>
+    <hyperlink ref="C232" r:id="rId224"/>
+    <hyperlink ref="C233" r:id="rId225"/>
+    <hyperlink ref="C234" r:id="rId226"/>
+    <hyperlink ref="C235" r:id="rId227"/>
+    <hyperlink ref="C236" r:id="rId228"/>
+    <hyperlink ref="C237" r:id="rId229"/>
+    <hyperlink ref="C238" r:id="rId230"/>
+    <hyperlink ref="C239" r:id="rId231"/>
+    <hyperlink ref="C240" r:id="rId232"/>
+    <hyperlink ref="C241" r:id="rId233"/>
+    <hyperlink ref="C242" r:id="rId234"/>
+    <hyperlink ref="C243" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="C244" r:id="rId236"/>
+    <hyperlink ref="C245" r:id="rId237"/>
+    <hyperlink ref="C246" r:id="rId238"/>
+    <hyperlink ref="C247" r:id="rId239"/>
+    <hyperlink ref="C248" r:id="rId240"/>
+    <hyperlink ref="C249" r:id="rId241"/>
+    <hyperlink ref="C250" r:id="rId242"/>
+    <hyperlink ref="C251" r:id="rId243"/>
+    <hyperlink ref="C252" r:id="rId244"/>
+    <hyperlink ref="C253" r:id="rId245"/>
+    <hyperlink ref="C254" r:id="rId246"/>
+    <hyperlink ref="C255" r:id="rId247"/>
+    <hyperlink ref="C256" r:id="rId248"/>
+    <hyperlink ref="C257" r:id="rId249"/>
+    <hyperlink ref="C258" r:id="rId250"/>
+    <hyperlink ref="C259" r:id="rId251"/>
+    <hyperlink ref="C260" r:id="rId252"/>
+    <hyperlink ref="C261" r:id="rId253"/>
+    <hyperlink ref="C262" r:id="rId254"/>
+    <hyperlink ref="C263" r:id="rId255"/>
+    <hyperlink ref="C264" r:id="rId256"/>
+    <hyperlink ref="C265" r:id="rId257"/>
+    <hyperlink ref="C266" r:id="rId258"/>
+    <hyperlink ref="C267" r:id="rId259"/>
+    <hyperlink ref="C268" r:id="rId260"/>
+    <hyperlink ref="C269" r:id="rId261"/>
+    <hyperlink ref="C270" r:id="rId262"/>
+    <hyperlink ref="C271" r:id="rId263"/>
+    <hyperlink ref="C272" r:id="rId264"/>
+    <hyperlink ref="C273" r:id="rId265"/>
+    <hyperlink ref="C274" r:id="rId266"/>
+    <hyperlink ref="C275" r:id="rId267"/>
+    <hyperlink ref="C276" r:id="rId268"/>
+    <hyperlink ref="C277" r:id="rId269"/>
+    <hyperlink ref="C278" r:id="rId270"/>
+    <hyperlink ref="C279" r:id="rId271"/>
+    <hyperlink ref="C280" r:id="rId272"/>
+    <hyperlink ref="C281" r:id="rId273"/>
+    <hyperlink ref="C282" r:id="rId274"/>
+    <hyperlink ref="C283" r:id="rId275"/>
+    <hyperlink ref="C284" r:id="rId276"/>
+    <hyperlink ref="C285" r:id="rId277"/>
+    <hyperlink ref="C286" r:id="rId278"/>
+    <hyperlink ref="C287" r:id="rId279"/>
+    <hyperlink ref="C288" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="C289" r:id="rId281"/>
+    <hyperlink ref="C290" r:id="rId282"/>
+    <hyperlink ref="C291" r:id="rId283"/>
+    <hyperlink ref="C292" r:id="rId284"/>
+    <hyperlink ref="C293" r:id="rId285"/>
+    <hyperlink ref="C294" r:id="rId286"/>
+    <hyperlink ref="C295" r:id="rId287"/>
+    <hyperlink ref="C296" r:id="rId288"/>
+    <hyperlink ref="C297" r:id="rId289"/>
+    <hyperlink ref="C298" r:id="rId290"/>
+    <hyperlink ref="C299" r:id="rId291"/>
+    <hyperlink ref="C300" r:id="rId292"/>
+    <hyperlink ref="C301" r:id="rId293"/>
+    <hyperlink ref="C302" r:id="rId294"/>
+    <hyperlink ref="C303" r:id="rId295"/>
+    <hyperlink ref="C304" r:id="rId296"/>
+    <hyperlink ref="C305" r:id="rId297"/>
+    <hyperlink ref="C306" r:id="rId298"/>
+    <hyperlink ref="C307" r:id="rId299"/>
+    <hyperlink ref="C308" r:id="rId300"/>
+    <hyperlink ref="C309" r:id="rId301"/>
+    <hyperlink ref="C310" r:id="rId302"/>
+    <hyperlink ref="C311" r:id="rId303"/>
+    <hyperlink ref="C312" r:id="rId304"/>
+    <hyperlink ref="C313" r:id="rId305"/>
+    <hyperlink ref="C314" r:id="rId306"/>
+    <hyperlink ref="C315" r:id="rId307"/>
+    <hyperlink ref="C316" r:id="rId308"/>
+    <hyperlink ref="C317" r:id="rId309"/>
+    <hyperlink ref="C318" r:id="rId310"/>
+    <hyperlink ref="C319" r:id="rId311"/>
+    <hyperlink ref="C320" r:id="rId312"/>
+    <hyperlink ref="C321" r:id="rId313"/>
+    <hyperlink ref="C322" r:id="rId314"/>
+    <hyperlink ref="C323" r:id="rId315"/>
+    <hyperlink ref="C324" r:id="rId316"/>
+    <hyperlink ref="C325" r:id="rId317"/>
+    <hyperlink ref="C326" r:id="rId318"/>
+    <hyperlink ref="C327" r:id="rId319"/>
+    <hyperlink ref="C328" r:id="rId320"/>
+    <hyperlink ref="C329" r:id="rId321"/>
+    <hyperlink ref="C330" r:id="rId322"/>
+    <hyperlink ref="C331" r:id="rId323"/>
+    <hyperlink ref="C332" r:id="rId324"/>
+    <hyperlink ref="C333" r:id="rId325"/>
+    <hyperlink ref="C335" r:id="rId326"/>
+    <hyperlink ref="C336" r:id="rId327"/>
+    <hyperlink ref="C337" r:id="rId328"/>
+    <hyperlink ref="C338" r:id="rId329"/>
+    <hyperlink ref="C339" r:id="rId330"/>
+    <hyperlink ref="C340" r:id="rId331"/>
+    <hyperlink ref="C341" r:id="rId332"/>
+    <hyperlink ref="C342" r:id="rId333"/>
+    <hyperlink ref="C343" r:id="rId334"/>
+    <hyperlink ref="C344" r:id="rId335"/>
+    <hyperlink ref="C345" r:id="rId336"/>
+    <hyperlink ref="C346" r:id="rId337"/>
+    <hyperlink ref="C347" r:id="rId338"/>
+    <hyperlink ref="C348" r:id="rId339"/>
+    <hyperlink ref="C349" r:id="rId340"/>
+    <hyperlink ref="C350" r:id="rId341"/>
+    <hyperlink ref="C351" r:id="rId342"/>
+    <hyperlink ref="C352" r:id="rId343"/>
+    <hyperlink ref="C353" r:id="rId344"/>
+    <hyperlink ref="C354" r:id="rId345"/>
+    <hyperlink ref="C355" r:id="rId346"/>
+    <hyperlink ref="C356" r:id="rId347"/>
+    <hyperlink ref="C357" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="C358" r:id="rId349"/>
+    <hyperlink ref="C359" r:id="rId350"/>
+    <hyperlink ref="C360" r:id="rId351"/>
+    <hyperlink ref="C361" r:id="rId352"/>
+    <hyperlink ref="C362" r:id="rId353"/>
+    <hyperlink ref="C363" r:id="rId354"/>
+    <hyperlink ref="C364" r:id="rId355"/>
+    <hyperlink ref="C365" r:id="rId356"/>
+    <hyperlink ref="C366" r:id="rId357"/>
+    <hyperlink ref="C367" r:id="rId358"/>
+    <hyperlink ref="C368" r:id="rId359"/>
+    <hyperlink ref="C369" r:id="rId360"/>
+    <hyperlink ref="C370" r:id="rId361"/>
+    <hyperlink ref="C371" r:id="rId362"/>
+    <hyperlink ref="C372" r:id="rId363"/>
+    <hyperlink ref="C374" r:id="rId364"/>
+    <hyperlink ref="C373" r:id="rId365"/>
+    <hyperlink ref="C375" r:id="rId366"/>
+    <hyperlink ref="C376" r:id="rId367"/>
+    <hyperlink ref="C377" r:id="rId368"/>
+    <hyperlink ref="C378" r:id="rId369"/>
+    <hyperlink ref="C379" r:id="rId370"/>
+    <hyperlink ref="C380" r:id="rId371"/>
+    <hyperlink ref="C381" r:id="rId372"/>
+    <hyperlink ref="C382" r:id="rId373"/>
+    <hyperlink ref="C383" r:id="rId374"/>
+    <hyperlink ref="C384" r:id="rId375"/>
+    <hyperlink ref="C385" r:id="rId376"/>
+    <hyperlink ref="C386" r:id="rId377"/>
+    <hyperlink ref="C387" r:id="rId378"/>
+    <hyperlink ref="C388" r:id="rId379"/>
+    <hyperlink ref="C389" r:id="rId380"/>
+    <hyperlink ref="C390" r:id="rId381"/>
+    <hyperlink ref="C391" r:id="rId382"/>
+    <hyperlink ref="C392" r:id="rId383"/>
+    <hyperlink ref="C393" r:id="rId384"/>
+    <hyperlink ref="C394" r:id="rId385"/>
+    <hyperlink ref="C395" r:id="rId386"/>
+    <hyperlink ref="C396" r:id="rId387"/>
+    <hyperlink ref="C397" r:id="rId388"/>
+    <hyperlink ref="C398" r:id="rId389"/>
+    <hyperlink ref="C399" r:id="rId390"/>
+    <hyperlink ref="C400" r:id="rId391"/>
+    <hyperlink ref="C401" r:id="rId392"/>
+    <hyperlink ref="C402" r:id="rId393"/>
+    <hyperlink ref="C403" r:id="rId394"/>
+    <hyperlink ref="C404" r:id="rId395"/>
+    <hyperlink ref="C405" r:id="rId396"/>
+    <hyperlink ref="C406" r:id="rId397"/>
+    <hyperlink ref="C407" r:id="rId398"/>
+    <hyperlink ref="C408" r:id="rId399"/>
+    <hyperlink ref="C409" r:id="rId400"/>
+    <hyperlink ref="C410" r:id="rId401"/>
+    <hyperlink ref="C411" r:id="rId402"/>
+    <hyperlink ref="C412" r:id="rId403"/>
+    <hyperlink ref="C413" r:id="rId404"/>
+    <hyperlink ref="C414" r:id="rId405"/>
+    <hyperlink ref="C415" r:id="rId406"/>
+    <hyperlink ref="C416" r:id="rId407"/>
+    <hyperlink ref="C417" r:id="rId408"/>
+    <hyperlink ref="C418" r:id="rId409"/>
+    <hyperlink ref="C419" r:id="rId410"/>
+    <hyperlink ref="C420" r:id="rId411"/>
+    <hyperlink ref="C421" r:id="rId412"/>
+    <hyperlink ref="C422" r:id="rId413"/>
+    <hyperlink ref="C423" r:id="rId414"/>
+    <hyperlink ref="C425" r:id="rId415"/>
+    <hyperlink ref="C424" r:id="rId416"/>
+    <hyperlink ref="C426" r:id="rId417"/>
+    <hyperlink ref="C427" r:id="rId418"/>
+    <hyperlink ref="C428" r:id="rId419"/>
+    <hyperlink ref="C429" r:id="rId420"/>
+    <hyperlink ref="C430" r:id="rId421"/>
+    <hyperlink ref="C431" r:id="rId422"/>
+    <hyperlink ref="C432" r:id="rId423"/>
+    <hyperlink ref="C433" r:id="rId424"/>
+    <hyperlink ref="C434" r:id="rId425"/>
+    <hyperlink ref="C435" r:id="rId426"/>
+    <hyperlink ref="C436" r:id="rId427"/>
+    <hyperlink ref="C443" r:id="rId428"/>
+    <hyperlink ref="C442" r:id="rId429"/>
+    <hyperlink ref="C441" r:id="rId430"/>
+    <hyperlink ref="C440" r:id="rId431"/>
+    <hyperlink ref="C439" r:id="rId432"/>
+    <hyperlink ref="C438" r:id="rId433"/>
+    <hyperlink ref="C437" r:id="rId434"/>
+    <hyperlink ref="C444" r:id="rId435"/>
+    <hyperlink ref="C445" r:id="rId436"/>
+    <hyperlink ref="C446" r:id="rId437"/>
+    <hyperlink ref="C447" r:id="rId438"/>
+    <hyperlink ref="C448" r:id="rId439"/>
+    <hyperlink ref="C449" r:id="rId440"/>
+    <hyperlink ref="C450" r:id="rId441"/>
+    <hyperlink ref="C453" r:id="rId442"/>
+    <hyperlink ref="C451" r:id="rId443"/>
+    <hyperlink ref="C452" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="C334" r:id="rId445"/>
+    <hyperlink ref="C2" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId447"/>

</xml_diff>

<commit_message>
334. Search in a Maze
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B330" workbookViewId="0">
-      <selection activeCell="D336" sqref="D336"/>
+    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
+      <selection activeCell="D339" sqref="D339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -6568,8 +6568,8 @@
       <c r="C337" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="D337" s="4" t="s">
-        <v>4</v>
+      <c r="D337" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="21">
@@ -6582,8 +6582,8 @@
       <c r="C338" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="D338" s="4" t="s">
-        <v>4</v>
+      <c r="D338" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="339" spans="1:4" ht="21">
@@ -6596,8 +6596,8 @@
       <c r="C339" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="D339" s="4" t="s">
-        <v>4</v>
+      <c r="D339" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="340" spans="1:4" ht="21">

</xml_diff>

<commit_message>
338. Making wired Connections
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A332" workbookViewId="0">
-      <selection activeCell="D339" sqref="D339"/>
+    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="D343" sqref="D343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -6610,8 +6610,8 @@
       <c r="C340" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="D340" s="4" t="s">
-        <v>4</v>
+      <c r="D340" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="341" spans="1:4" ht="21">
@@ -6624,8 +6624,8 @@
       <c r="C341" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="D341" s="4" t="s">
-        <v>4</v>
+      <c r="D341" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="342" spans="1:4" ht="21">
@@ -6638,8 +6638,8 @@
       <c r="C342" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="D342" s="4" t="s">
-        <v>4</v>
+      <c r="D342" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="343" spans="1:4" ht="21">
@@ -6652,8 +6652,8 @@
       <c r="C343" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="D343" s="4" t="s">
-        <v>4</v>
+      <c r="D343" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="21">

</xml_diff>

<commit_message>
439. Count set bits in an integer
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="D343" sqref="D343"/>
+    <sheetView tabSelected="1" topLeftCell="B440" workbookViewId="0">
+      <selection activeCell="D444" sqref="D444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -8066,8 +8066,8 @@
       <c r="C444" s="6" t="s">
         <v>454</v>
       </c>
-      <c r="D444" s="4" t="s">
-        <v>4</v>
+      <c r="D444" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="445" spans="1:4" ht="21">

</xml_diff>

<commit_message>
440. Find the two non-repeating elements in an array of repeating elements
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1886,8 +1886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B440" workbookViewId="0">
-      <selection activeCell="D444" sqref="D444"/>
+    <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
+      <selection activeCell="D445" sqref="D445"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -8080,8 +8080,8 @@
       <c r="C445" s="6" t="s">
         <v>455</v>
       </c>
-      <c r="D445" s="4" t="s">
-        <v>4</v>
+      <c r="D445" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="446" spans="1:4" ht="21">

</xml_diff>

<commit_message>
444. Find position of the only set bit
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1887,7 +1887,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
-      <selection activeCell="D445" sqref="D445"/>
+      <selection activeCell="C449" sqref="C449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -8094,8 +8094,8 @@
       <c r="C446" s="6" t="s">
         <v>456</v>
       </c>
-      <c r="D446" s="4" t="s">
-        <v>4</v>
+      <c r="D446" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="447" spans="1:4" ht="21">
@@ -8108,8 +8108,8 @@
       <c r="C447" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="D447" s="4" t="s">
-        <v>4</v>
+      <c r="D447" s="12" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="448" spans="1:4" ht="21">
@@ -8122,8 +8122,8 @@
       <c r="C448" s="6" t="s">
         <v>458</v>
       </c>
-      <c r="D448" s="4" t="s">
-        <v>4</v>
+      <c r="D448" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="449" spans="1:4" ht="21">
@@ -8136,8 +8136,8 @@
       <c r="C449" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="D449" s="4" t="s">
-        <v>4</v>
+      <c r="D449" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="450" spans="1:4" ht="21">

</xml_diff>

<commit_message>
445. Copy set bits in a range
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -1887,7 +1887,7 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A438" workbookViewId="0">
-      <selection activeCell="C449" sqref="C449"/>
+      <selection activeCell="D450" sqref="D450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -8150,8 +8150,8 @@
       <c r="C450" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="D450" s="4" t="s">
-        <v>4</v>
+      <c r="D450" s="11" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="451" spans="1:4" ht="21">

</xml_diff>

<commit_message>
1828. Queries on Number of Points Inside a Circle
</commit_message>
<xml_diff>
--- a/babbar.xlsx
+++ b/babbar.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive - KLK VENTURES PRIVATE LIMITED\Desktop\CP-Solving-Streak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\CP-Solving-Streak\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1896,18 +1896,18 @@
   <dimension ref="A1:D453"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A339" workbookViewId="0">
-      <selection activeCell="D344" sqref="D344"/>
+      <selection activeCell="D346" sqref="D346"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="26.58203125" customWidth="1"/>
-    <col min="3" max="3" width="94.25" customWidth="1"/>
+    <col min="2" max="2" width="26.59765625" customWidth="1"/>
+    <col min="3" max="3" width="94.19921875" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25">
+    <row r="1" spans="1:4" ht="24.6">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>